<commit_message>
1. Add loging and minor changes to load_new_data.py script 2. Add dockerfile and configurations to run script and postgre in containers
</commit_message>
<xml_diff>
--- a/notebooks/new_articles_df.xlsx
+++ b/notebooks/new_articles_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,30 +483,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>The $8 billion Sam Bankman-Fried criminal trial starts today — here's what's at stake and how we got here</t>
+          <t>Sam Bankman-Fried heads for trial on charges of stealing billions from FTX users</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>watch now
-A year ago, Sam Bankman-Fried was revered as a titan of the industry and living large at a $40 million penthouse in the Bahamas, while he ran a crypto empire valued at $32 billion. On Tuesday morning in a Manhattan federal court in New York, the now disgraced founder and ex-CEO of the bankrupt crypto exchange FTX will stand trial for allegedly masterminding one of the biggest financial frauds in U.S. history. Here is what you need to know about the multi-week trial that starts today, the government's case against 31-year-old Bankman-Fried, and how we got here.
-The trial(s) against Sam Bankman-Fried
-Tuesday marks the start of the first of two separate criminal trials against the man once celebrated as a titan of the industry. In the first trial, Bankman-Fried faces seven criminal counts related to the collapse of the crypto empire he built, including wire fraud, securities fraud and money laundering. A superseding indictment alleges that Bankman-Fried misused billions of dollars worth of customer money for personal purchases, including buying more than $200 million of upscale real estate properties in the Bahamas, as well as to cover bad bets made at his crypto hedge fund, Alameda Research. The government says customer cash was shuttled to Alameda via two channels: Users depositing cash directly into accounts held by Alameda and through a secret backdoor that was baked into FTX's code. Prosecutors from the Southern District of New York, who contend that more than $8 billion of customers' money has gone missing, also allege that Bankman-Fried defrauded FTX investors by covering up the scheme. The government has separately accused SBF of using customer funds to make more than $100 million in campaign contributions for the 2022 midterm elections. The full list of charges are: Conspiracy to commit wire fraud on customers of FTX.
-Wire fraud on customers of FTX.
-Conspiracy to commit wire fraud on lenders to Alameda Research.
-Wire fraud on lenders to Alameda Research.
-Conspiracy to commit fraud on customers of FTX in connection with purchase and sale of derivatives.
-Conspiracy to commit securities fraud on investors in FTX.
-Conspiracy to commit money laundering. A conviction on all counts could land him more than 100 years in prison. Bankman-Fried, who is the son of two Stanford legal scholars, has pleaded not guilty to all charges. Bankman-Fried's criminal trial is expected to last up to six weeks, and it kicks off at 9:30 a.m. ET on Tuesday with jury selection. From there, the prosecution will take roughly four weeks to lay out its case, and the defense will take another one to two weeks to present its side. It's not yet known whether Bankman-Fried will testify, but the witness roster is expected to include his top deputies at FTX and Alameda, who also happened to comprise his innermost social circle before his crypto empire imploded. The list of cooperating witnesses anticipated to take the stand include Bankman-Fried's ex-girlfriend, Caroline Ellison, and his ex-best friend from high school math camp and former MIT roommate, Gary Wang. Ellison, who is the former chief executive of Alameda Research, and FTX co-founder Wang, both pleaded guilty in December to multiple charges and have been cooperating with the U.S. attorney's office in Manhattan for months. Since August, Bankman-Fried has been held in a jail in Brooklyn, New York, after having his multimillion-dollar bail revoked for witness tampering, after allegedly leaking to The New York Times the private diary entries of Ellison, who is expected to be a star witness for the prosecution. Court documents filed so far indicate that lawyers for Bankman-Fried could present an "advice of counsel" defense. That's where they would say that he was following the guidance of FTX lawyers and didn't realize that what he was doing was illegal. Judge Lewis Kaplan has already ruled, however, that this defense strategy cannot be included in their opening remarks since it might risk prejudicing the jury from the start. A second criminal trial is slated for March 2024 that will deal with additional charges brought after Bankman-Fried's extradition to the U.S. from FTX's headquarters in the Bahamas.
-Samuel Bankman-Fried's poster in downtown San Francisco. MacKenzie Sigalos | CNBC
-How we got here
-The Kimchi Swap put Sam Bankman-Fried on the map. The year was 2017, and the ex-Jane Street Capital quant trader noticed something funny when he looked at the page on CoinMarketCap.com listing the price of bitcoin on exchanges around the world. Today, that price is pretty much uniform across the exchanges, but back then, Bankman-Fried previously told CNBC, he would sometimes see a 60% difference in the value of the coin. His immediate instinct, he said, was to get in on the arbitrage trade — buying bitcoin on one exchange, selling it back on another exchange, and then earning a profit equivalent to the price spread. "That's the lowest hanging fruit," Bankman-Fried said in September. The arbitrage opportunity was especially compelling in South Korea, where the exchange-listed price of bitcoin was significantly more than in other countries. It was dubbed the Kimchi Premium — a reference to the traditional Korean side dish of salted and fermented cabbage. After a month of personally dabbling in the market, Bankman-Fried launched his own trading house, Alameda Research — named after his hometown of Alameda, California, near San Francisco — to scale the opportunity and work on it full time. Bankman-Fried said in an interview with CNBC that the firm sometimes made as much as a million dollars a day. Part of why SBF earned street cred for carrying out a relatively straightforward trading strategy was because it wasn't the easiest thing to execute on crypto rails five years ago. Bitcoin arbitrage involved setting up connections to each one of the trading platforms, as well as building out other complicated infrastructure to abstract away a lot of the operational aspects of making the trade. Bankman-Fried's Alameda became very good at that, and the money rolled in. From there, the SBF empire ballooned. Alameda's success spurred the launch of crypto exchange FTX. In April 2019, Bankman-Fried and Wang — along with University of California, Berkeley, graduate Nishad Singh — founded FTX.com, an international cryptocurrency exchange that offered customers innovative trading features, a responsive platform and a reliable experience. FTX's success begat a $2 billion venture fund that seeded other crypto firms. Bankman-Fried's personal wealth grew to around $26 billion at its peak. Bankman-Fried was suddenly the poster boy for crypto everywhere, and the FTX logo adorned everything from Formula One race cars to a Miami basketball arena. He went on an endless press tour, bragged about having a balance sheet that could one day buy Goldman Sachs, and became a fixture in Washington, where he was one of the Democratic Party's top donors, promising to sink $1 billion into U.S. political races before later backtracking. It was all a mirage. As crypto prices tanked in 2022, Bankman-Fried boasted that he and his enterprise were immune. But in fact, the sectorwide wipeout hit his operation quite hard. Alameda borrowed money to invest in failing digital asset firms in the spring and summer of 2022 to keep the industry afloat, then reportedly siphoned off FTX customers' deposits to stave off margin calls and meet immediate debt obligations. A fight on Twitter, now known as X, with the CEO of rival exchange Binance pulled the mask off the scheme. Alameda, FTX and a host of subsidiaries Bankman-Fried founded filed for bankruptcy protection in Delaware. Bankman-Fried lost 94% of his personal wealth in a single day; was arrested in the Bahamas; was subsequently extradited to the U.S. and taken into custody; was released on a $250 million bail to his parents' California home; and then later remanded back into custody for alleged witness tampering. Meanwhile, federal prosecutors and regulators have accused Bankman-Fried of not just having perpetrated a fraud, but having done so "from the start," according to a filing from the Securities Exchange Commission. SEC and Commodity Futures Trading Commission regulators, alongside federal prosecutors from the United States Attorney's Office for the Southern District of New York, say that Bankman-Fried was at the heart — indeed, the driver — of "one of the biggest financial frauds in American history," in the words of U.S. Attorney Damian Williams. Federal regulators at the CFTC say that just a month after founding FTX.com, Bankman-Fried, "unbeknownst to all but a small circle of insiders," was leveraging customer assets — specifically, customers' personal cryptocurrency deposits — for Alameda's own bets. Rehypothecation is the term for when businesses legally use customer assets to speculate and invest. But Bankman-Fried didn't have permission from customers to gamble with their funds. FTX's own terms of use specifically forbade him, or Alameda, from using customer money for anything — unless the customer allowed it. And from FTX's inception, there was a lot of customer money. The CFTC cited 2019 reports from FTX which pegged the futures volume alone as often exceeding $100 million every day. Using customer money for Alameda's bets constituted fraud, the CFTC alleges. From the very genesis of FTX, regulators allege, Bankman-Fried was using customer funds to bankroll his speculative investments. It was a steep fall from hero to villain. But there were a lot of signs.
-watch now
-A lousy crypto hedge fund
-Despite the deck being stacked in Alameda's favor, the hedge fund offered terrible returns. A court filing indicated that Alameda lost more than $3.7 billion over its lifetime, despite public statements by FTX leaders touting how profitable the trading arm was. Alameda's losses and lending structure were a critical component of FTX's eventual collapse. Alameda didn't just allegedly play fast and loose with customer money. The hedge fund borrowed aggressively from multiple lenders, including Voyager Digital and BlockFi Lending. Both those companies entered Chapter 11 bankruptcy proceedings in 2022, and FTX targeted both for acquisition. Alameda secured its loans from Voyager and BlockFi with FTT tokens, which FTX minted itself. Bankman-Fried's empire controlled the vast majority of the available currency, with only a small amount of FTT actually circulating at any time. Alameda should have acknowledged the fact that its tokens couldn't be sold at the price that they claimed they were worth, the CFTC alleges in its complaint. This was because any attempt by Alameda to sell off their FTT tokens would crater FTT's price, given how much of the available supply Alameda controlled. Instead of correctly marking its tokens to market, though, Alameda marked their entire hoard of FTT at the prevailing market price. Alameda used this methodology with other coins as well, including Solana and Serum (a token created and promoted by FTX and Alameda), using them to collateralize billions in loans to other crypto players. Industry insiders even had a nickname for those tokens — "Sam coins." The tables began to turn in May 2022 after the collapse of Luna, a stablecoin whose implosion and subsequent crash devastated other lenders and crypto firms and sent crypto prices plunging. Major Alameda lenders, like Voyager, declared bankruptcy. Remaining lenders began to execute margin calls or liquidate open positions with customers, including Alameda. The CFTC alleges that between May and June 2022, Alameda was subjected to "a large number of margin calls and loan recalls." Unbeknownst to investors, lenders, or regulators, Alameda lacked enough liquid assets to service its loan obligations. But while Alameda was illiquid, FTX's customers — who had been constantly reassured that the exchange, and Bankman-Fried, were determined to protect their interests — were not.
-watch now
-The fraud — exposed
-Bankman-Fried stepped down from his leadership position at Alameda Research in Oct. 2021 in what CFTC regulators claim was a calculated bid to cultivate a false sense of separation between FTX and the hedge fund. But he continued to exercise control, regulators claim. Bankman-Fried allegedly ordered Alameda to increase its use of customer assets, drawing down massively on its "unlimited" credit line at FTX. "Alameda was able to rely on its undisclosed ordinary-course access to FTX credit and customer funds to facilitate these large withdrawals, which were several billion dollars in notional value," the CFTC filing reads. By the middle of 2022, Alameda owed FTX's unwitting customers approximately $8 billion. Bankman-Fried had testified before the House that FTX boasted world-class risk management and compliance systems, but in reality, according to the firm's own bankruptcy filings, it possessed almost nothing in the way of record-keeping. Then, on Nov. 2, the first domino fell. Crypto trade publication CoinDesk publicized details on Alameda's balance sheet which showed $14.6 billion in assets. Over $7 billion of those assets were either FTT tokens or Bankman-Fried-backed coins like Solana or Serum. Another $2 billion were locked away in equity investments. For the first time ever, the secretive inner workings of Alameda Research were revealed to be a Potemkin village. Investors began to liquidate their FTT tokens and withdraw their holdings from FTX, a potentially calamitous situation for Bankman-Fried. Alameda still had billions of collateralized loans outstanding — but if the value of their collateral, FTT, fell too far, their lenders would execute further margin calls, demanding full repayment of loans. Allegedly, Alameda had already been unable to fulfill loan obligations over the summer without accessing customer funds. Now, with money flowing out of the exchange and FTT's price slipping, Alameda and FTX faced a liquidity crunch. In a now-deleted tweet, Bankman-Fried continued to claim FTX was fully funded and that customer assets were safe. But on Nov. 6, 2022, four days after the CoinDesk article, the crack widened into a chasm, thanks to an old investor-turned-rival, Changpeng "CZ" Zhao. Zhao founded Binance in 2017, and it was the first outside investor in FTX, funding a Series A round in 2019. FTX bought out Binance in 2021 with a combination of FTT and other coins, according to Zhao. Zhao dropped the hammer with a tweet saying that because of "recent revelations that have came [sic] to light, we have decided to liquidate any remaining FTT on our books." FTX executives scrambled to contain the damage, and Alameda traders managed to fend off outflows for two days, holding the price of FTT at around $22. Publicly, Bankman-Fried continued to operate as if all was well. "FTX is fine. Assets are fine," he wrote in a tweet on Nov. 7 that has since been deleted. But at the same time Bankman-Fried was tweeting reassurances, internally, executives were growing more and more alarmed at the increasing shortfall, according to prosecutors. Bankman-Fried and other executives admitted to each other that "FTX customer funds were irrevocably lost because Alameda had appropriated them." It was an admission that flew in the face of everything Bankman-Fried would claim publicly up through the day of his arrest, a month later. By Nov. 8, the shortfall had grown from $1 billion to $8 billion. Bankman-Fried had been courting outside investors for a rescue package, but everyone declined. FTX issued a pause on all customer withdrawals that day. FTT's price plummeted by over 75%. Bankman-Fried was in the midst of a high-tech, decentralized run on the bank. Out of options, he turned to Zhao, who announced that he'd signed a "non-binding" letter of intent to acquire FTX.com. But just a day later, on Nov. 9, Binance said it would not go through with the acquisition, citing reports of "mishandled customer funds" and federal investigations. Two days later, Bankman-Fried resigned as CEO of FTX and associated entities. FTX's longtime attorneys at Sullivan &amp; Cromwell approached John J. Ray, who oversaw Enron through its bankruptcy, to assume Bankman-Fried's former position. FTX filed for bankruptcy that same day, on Nov. 11, 2022. A month later, Bankman-Fried was arrested by Bahamian authorities, pending extradition on charges of fraud, conspiracy, and money laundering. Bankman-Fried, a devotee of a philosophy known as "effective altruism," was apparently driven by an obsessive need to quantify the impact he had on this world, measured in dollars and tokens. He drafted a spreadsheet which measured the influence that Alameda had on the planet (and determined it was nearly a net wash). Billions of dollars of customer money were left floating in venture funds, political war chests and charitable coffers, although John Ray's team has clawed back more than $7 billion so far. Almost a decade ago, Bankman-Fried posed a hypothetical question to his friends and family on his personal blog: Waxing poetic on effective altruism, he asked rhetorically, "Just how much impact can a dollar have?" "Well, if you want a one-sentence answer, here it is: one two thousandth of a life," he said. The CFTC alleges that over $8 billion of customer funds are missing. Some customers have doubtless lost their life savings, their kid's college funds, their future down payments. By Bankman-Fried's own math, his alleged misdeeds were worth four million lives. — CNBC's Rohan Goswami contributed to this report.</t>
+          <t>Companies Champion Trust Llc Follow
+NEW YORK, Oct 3 (Reuters) - Sam Bankman-Fried is set to go on trial on charges of stealing billions of dollars from customers of his FTX cryptocurrency exchange starting on Tuesday, nearly a year after the company's collapse shocked markets and tattered his reputation.
+Dozens of New York residents, many holding jury summonses in their hands, began streaming into a federal courthouse in lower Manhattan ahead of jury selection, which is scheduled to start at 9:30 a.m. EDT (1330 GMT).
+Federal prosecutors say the 31-year-old former billionaire embezzled from FTX customers since its founding in 2019 through its November 2022 bankruptcy in order to prop up his hedge fund Alameda Research, buy luxury properties and donate more than $100 million to U.S. political candidates.
+Bankman-Fried has pleaded not guilty to seven counts of fraud and conspiracy. He has acknowledged inadequate risk management, but denied stealing funds. His lawyers have signaled in court papers they plan to argue that FTX's treatment of customer funds were proper, and that others at FTX and Alameda bore the bulk of the blame for their failure.
+The first step in the trial will be selecting the 12-member jury that will ultimately weigh those competing narratives in deciding whether to convict Bankman-Fried.
+U.S. District Judge Lewis Kaplan will ask a pool of New York residents questions about their backgrounds and experiences in an effort to weed out any prospective jurors who may be biased.
+The trial is expected to last up to six weeks. It will feature testimony from three former members of Bankman-Fried's inner circle who have pleaded guilty to fraud charges themselves and agreed to cooperate with the Manhattan U.S. Attorney's office.
+Bankman-Fried's lawyers have signaled they plan to challenge the credibility of those witnesses - who include former Alameda chief Caroline Ellison and former FTX executives Gary Wang and Nishad Singh - by arguing they are motivated to implicate their client to get a lower sentence, a common strategy in white collar fraud cases.
+They have also laid the groundwork to argue that Bankman-Fried believed his exchange was allowed to invest customers' deposits as long as they were ultimately able to take out their funds, and that a series of business failures - not deliberate fraud - left the exchange without enough money to meet withdrawal requests.
+Bankman-Fried's is the highest profile case U.S. prosecutors have so far brought against a former cryptocurrency executive.
+His indictment last December marked a spectacular fall from grace for Bankman-Fried, who had garnered a reputation as a legitimate operator in an industry whose image was pockmarked by scams and purported get-rich-quick schemes.
+Prosecutors say Bankman-Fried built that reputation on lies and bolstered it with endorsements from celebrities and star athletes.
+Bankman-Fried has been detained at the Metropolitan Detention Center in Brooklyn since Aug. 11, after the judge found he had likely engaged in witness tampering - including by sharing Ellison's personal writings with a reporter. Ellison and Bankman-Fried are former romantic partners.
+He will be brought to court early on most days to allow him to prepare with his lawyers.
+Reporting by Jody Godoy and Luc Cohen in New York; Editing by Amy Stevens, Lincoln Feast and Nick Zieminski
+Our Standards: The Thomson Reuters Trust Principles.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -521,201 +519,259 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['Mackenzie Sigalos']</t>
+          <t>['Jody Godoy Luc Cohen', 'Jody Godoy', 'Luc Cohen', 'Thomson Reuters', 'Jody Godoy Reports On Banking', 'Securities Law. Reach Her At Jody.Godoy Thomsonreuters.Com', 'Reports On The New York Federal Courts. Previously Worked As A Correspondent In Venezuela', 'Cellino', 'Barnes Firms Battle Former Colleagues Over Fees', 'Years After Split']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.cnbc.com/2023/10/03/sam-bankman-fried-criminal-trial-starts-today-heres-whats-at-stake.html</t>
+          <t>https://www.reuters.com/legal/sam-bankman-fried-heads-trial-charges-stealing-billions-ftx-users-2023-10-03/</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://news.google.com/rss/articles/CBMiZ2h0dHBzOi8vd3d3LmNuYmMuY29tLzIwMjMvMTAvMDMvc2FtLWJhbmttYW4tZnJpZWQtY3JpbWluYWwtdHJpYWwtc3RhcnRzLXRvZGF5LWhlcmVzLXdoYXRzLWF0LXN0YWtlLmh0bWzSAWtodHRwczovL3d3dy5jbmJjLmNvbS9hbXAvMjAyMy8xMC8wMy9zYW0tYmFua21hbi1mcmllZC1jcmltaW5hbC10cmlhbC1zdGFydHMtdG9kYXktaGVyZXMtd2hhdHMtYXQtc3Rha2UuaHRtbA?oc=5</t>
+          <t>https://news.google.com/rss/articles/CBMia2h0dHBzOi8vd3d3LnJldXRlcnMuY29tL2xlZ2FsL3NhbS1iYW5rbWFuLWZyaWVkLWhlYWRzLXRyaWFsLWNoYXJnZXMtc3RlYWxpbmctYmlsbGlvbnMtZnR4LXVzZXJzLTIwMjMtMTAtMDMv0gEA?oc=5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.cnbc.com</t>
+          <t>https://www.reuters.com</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>CNBC</t>
+          <t>Reuters</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The ‘wild bunch’ have taken control of the bond market. Here’s where they could wreak havoc next.</t>
+          <t>The 6 wildest details about Sam Bankman-Fried that Michael Lewis revealed in a tell-all interview</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The bond market is front and center for investors these days, with JPMorgan warning of a “financial accident” if yields keep going up, driving prices lower.
-“The damage in bonds has been more severe and more sustained than for equities, and you can’t help wondering where the real damage is. You can’t have this much value destruction in bonds without there being some stress somewhere. However, it’s near impossible to work out where exactly it might come to the surface and on the heels of the worst month for bonds of the year,” noted a team of Deutsche Bank strategists led by Jim Reid on Monday.
-Our call of the day from Ed Yardeni, president of Yardeni Research, offers an idea on the next market to fall. That’s as he raises the alarm over what he calls the “Wild Bunch,” or bond vigilantes, who have “seized control of the Treasury market.” His hope is that cooling inflation will calm things down.
-In a note to clients, Yardeni ticks off evidence of those bond vigilantes in action. For starters, the fact that the 10-year Treasury yield BX:TMUBMUSD10Y rose on recent weak data instead of declining suggests a “shift in bond investors’ focused from what monetary policy makers may do to rising alarm about what fiscal policy makers are doing.”
-“The worry is that the escalating federal budget deficit will create more supply of bonds than demand can meet, requiring higher yields to clear the market; that worry has been the bond vigilantes’ entrance cue,” he says.
-Yardeni also sees the vigilantes in action when it comes to yield curve disinversion lately — an inverted yield curve occurs when interest paid on short-term debt is more than that of longer term bonds.
-“Perversely, now that the Fed seems to be on the verge of terminating its rate hiking, bond investors might have concluded that short-term rates aren’t high enough to cause a financial crisis, credit crunch, and a recession,” he said.
-And here’s where he’s on guard for trouble, as he notes that the wild bunch have oddly left the high-yield corporate debt market — flat and stable –alone:
-“Could it be that some of them view the government’s securities as riskier than high-yield corporates? The result of their rampage in the Treasury market suggests as much,” he said, adding that they are on alert for signs of rampage spreading to high yields.
-And for sure, the wild bunch have DC policy makers in their sights, after causing the Treasury market to fully reverse a drop in the 10-year yield from the global financial crisis through the pandemic over the past three years, he notes.
-Their message is clear, says Yardeni: “Take meaningful actions to reduce the federal deficit now and in the future or we will push the bond yield up to whatever level it takes to get you to do so!”
-Read: How Treasury market upheaval is rippling through global markets in 4 charts
-The markets
-Stock futures ES00, -0.53% NQ00, -0.69% are pointing to opening losses, with the yield on the 10-year Treasury note BX:TMUBMUSD10Y up 4 basis points and that of the 30-year BX:TMUBMUSD30Y up 7 basis points. The dollar DXY is up, notably against the Russian ruble USDRUB, +0.73% , while gold GC00, -0.28% , silver SI00, -0.87% and oil CL.1, -0.59% are under pressure.
-Read: Gold appears headed for a ‘death cross’ just 5 months after teasing record highs
-For more market updates plus actionable trade ideas for stocks, options and crypto, subscribe to MarketDiem by Investor’s Business Daily.
-The buzz
-POINT Biopharma PNT, +0.22% stock is up 84% after Eli Lilly announced a $1.4 billion deal for the cancer treatment company, paying $12.50 a share.
-SmileDirectClub shares SDC, -61.18% are down another 12% following a bankruptcy filing, as a buyer for the teeth straightening group could be hard to find.
-WeWork stock WE, -1.99% is down 5% after the office work space provider said it would miss interest payments to continue talks with its lenders.
-U.S.-listed Chinese stocks are down after property developers (except Evergrande, which rallied) pulled the Hang Seng HK:HSI 2.6% lower. Alibaba BABA, -0.24% , JD.com JD, -0.21% , XPeng XPEV, -1.25% and Li Auto LI, -1.29% are off 2% or more.
-Tesla TSLA, +0.55% has launched a less expensive, rear-wheel-drive version of its bestselling Model Y crossover SUV in the U.S.
-Cleveland Fed President Loretta Mester said late Monday that the central bank may need to hike rates once more this year and then keep them high “for some time.”
-Elsewhere a speech is due from Atlanta Fed President Raphael Bostic at 8 a.m., followed by job openings at 10 a.m.
-Best of the web
-Why home insurance prices in the U.S. went up 21% between 2022 and 2023.
-Meta plans to charge $14 a month for ad-free Instagram or Facebook.
-Burger King is still open in Russia despite a pledge to exit.
-The chart
-Here’s a chart from the portfolio manager of Crescat Capital, Otavio Costa, whose chart sums up possible brewing trouble for tech companies:
-@TaviCosta
-The tickers
-These were the top-searched tickers on MarketWatch as of 6 a.m.:
-Random reads
-On the toilet? Stay off your phone.
-NASA has a serious plan to build houses on the moon.
-In bedbug-plagued Paris, hotels will cost 300% more for the 2024 Olympics
-Need to Know starts early and is updated until the opening bell, but sign up here to get it delivered once to your email box. The emailed version will be sent out at about 7:30 a.m. Eastern.
-Listen to the Best New Ideas in Money podcast with MarketWatch financial columnist James Rogers and economist Stephanie Kelton.</t>
+          <t>Michael Lewis gave a peek into details from his new book on Sam Bankman-Fried in a tell-all interview.
+"The Big Short" author said he had over 100 meetings with Bankman-Fried.
+Lewis said SBF was friends with Tom Brady and once considered paying Donald Trump not to run in 2024.
+NEW LOOK Sign up to get the inside scoop on today’s biggest stories in markets, tech, and business — delivered daily. Read preview Loading Something is loading. Thanks for signing up! Access your favorite topics in a personalized feed while you're on the go. download the app Email address Sign up By clicking “Sign Up”, you accept our Terms of Service and Privacy Policy . You can opt-out at any time.
+Advertisement
+Advertisement
+"The Big Short" author Michael Lewis shared some of the wildest details from his forthcoming book on disgraced FTX cofounder Sam Bankman-Fried during a tell-all interview with "60 Minutes" on Sunday.
+Lewis said he met with Bankman-Fried more than 100 times over the course of two years — and had a front row seat to FTX's historic collapse. Lewis's book, "Going Infinite: The Rise and Fall of. New Tycoon," hit shelves today — the same day Bankman-Fried's criminal trial will kick off in New York.
+Here are six of the wildest stories from Lewis' interview:
+SBF wanted to pay Donald Trump not to run for office
+The biographer said Bankman-Fried, who at one point was worth $26 billion on paper, looked into how much it would cost to pay the former president not to run in the 2024 presidential election.
+Advertisement
+Advertisement
+"There was a number that was kicking around," Lewis said during the "60 Minutes" interview. "The number that was kicking around when I was talking to Sam about this was $5 billion."
+President Donald Trump sits at the Resolute Desk in May 2020. Erin Schaff-Pool/Getty Images
+The author added that Bankman-Fried wasn't sure whether the figure had come directly from Trump, and a spokesperson for Trump told Insider's Lloyd Lee that SBF has been "outed as a fraudster and someone that can't be trusted."
+Lewis said Bankman-Fried viewed Trump as an "existential threat" because of Trump's efforts to undermine the 2020 election.
+Tom Brady once 'adored' Bankman-Fried
+The former NFL player and SBF had an authentic relationship, according to Lewis.
+Advertisement
+Advertisement
+"Tom Brady, I think, adored him," Lewis said. "Tom Brady thought he was a really interesting person. I think he liked to hear what he had to say."
+The author added that Bankman-Fried also "really liked" Brady.
+Tom Brady and Sam Bankman-Fried had an unlikely friendship, according to Michael Lewis. Sebastian Widmann/Getty Images
+"And Sam wasn't a big sports person," Lewis said. "So it was funny to watch that interaction. It was like, 'These two people actually get along.' It's like the class nerd and the quarterback."
+SBF paid Brady $55 million to help promote his crypto exchange platform for 20 hours a year over the course of three years, Lewis said, adding that the ex-quarterback was "crushed" when FTX collapsed.
+Advertisement
+Advertisement
+"I think as time has gone by — and he's ceased to get a really good explanation about what's happened — I think he's just like, 'He tricked me. I'm angry. I don't want to have anything to do with it anymore,'" Lewis said of Brady's reaction.
+A representative for Brady did not immediately respond to a request for comment.
+FTX also shelled out millions for Larry David and Steph Curry's commercials
+FTX paid Larry David $10 million for his role in FTX's Super Bowl commercial, while Steph Curry got $35 million for a similar deal to Brady's, Lewis said.
+The author said Bankman-Fried's heavy spending — including spending over $100 million for the naming rights to the Miami Heat's arena — made him popular among some of the biggest names in Hollywood and sports.
+Advertisement
+Advertisement
+Vogue editor-in-chief Anna Wintour attends the 2022 Met Gala. Matt Winkelmeyer/MG22/Getty Images
+Vogue's Anna Wintour even reached out to SBF to attempt to get him to sponsor the Met Gala, but the former FTX CEO had no idea who she was, Lewis told "60 Minutes." The author added that he found it strange that a style icon like Wintour wanted to work with Bankman-Fried — who he dubbed "the worst-dressed person in America."
+"It was a social experiment: The person who has nothing all of a sudden has seemingly infinite dollars, will give it away, is unbelievably open-handed about it, and doesn't ask a whole lot of questions," Lewis said. "Who shows up when this person exists? Everybody, everybody comes to the trough. Everybody wants to be his best friend."
+However, since FTX's collapse and the fraud charges that followed, Lewis said SBF has "no friends."
+Spokespeople for David, Curry, and Wintour did not immediately respond to a request for comment.
+Advertisement
+Advertisement
+SBF played a video game during his first live TV interview
+Lewis said Bankman was pretty nonchalant about his first interview on live television. According to the author, SBF wore cargo shorts and had his signature ruffled hair.
+Sam Bankman-Fried, a known "League of Legends" fan, played a video game during his first live TV interview, Michael Lewis said. Riot Games
+"If you watch the clip you can see his eyes going back and forth, back and forth," Lewis said. "It's because he's trying to win his video game at the same time he's on the air."
+The FTX cofounder is known to be an avid gamer and reportedly played "League of Legends" during a pitch meeting with Sequoia Capital investors.
+SBF 'may go mad' without internet access
+Bankman-Fried doesn't stop at at video games. He also needs a "constant stream of information," Lewis said.
+Advertisement
+Advertisement
+"Now that sounds crazy, but I do think that if he had the internet, he could survive jail forever," Lewis said. "Without having a constant stream of information to react to — I think he may go mad."
+Sam Bankman-Fried. Michael M. Santiago/Getty Images
+SBF's greatest fear when it comes to the prospect of going to prison over his fraud charges is that he might lose access to the internet, the author said.
+"If you gave Sam Bankman-Fried a choice — this is quite serious — of living in a $39 million penthouse in the Bahamas without the internet, or the Metropolitan Detention Center in Brooklyn with the internet, there's no question in my mind he'd take the jail," Lewis said.
+Lewis said he believes SBF 'had a great business'
+"They actually had a great, real business," Lewis told "60 Minutes." "If no one had cast aspersions on the business, if there hadn't been a run on customer deposits, they'd still be sitting there making tons of money."
+Advertisement
+Advertisement
+The author said he didn't feel it was accurate to compare Bankman-Fried to the likes of other famous scammers like Bernie Madoff or Elizabeth Holmes.
+"It's a little different than supplying phony medical information to people that might kill them," Lewis said when the interviewer compared SBF to the disgraced Theranos founder. "In this case what you're doing is possibly losing some money that belonged to crypto speculators in the Bahamas. On the other hand, this is not to excuse. He shouldn't have done that."
+Bankman-Fried has been accused of fleecing customers and investors of billions of dollars.
+Prosecutors in the criminal trial against SBF allege FTX borrowed money from customer accounts to fund bets through Alameda Research, its affiliated hedge fund. He directed employees to develop programming code that allowed unlimited funds to move between the companies quickly and quietly, prosecutors said in their indictment.
+Advertisement
+Advertisement
+Michael Lewis said he couldn't compare SBF to scammers like Bernie Madoff. Jim Spellman/WireImage
+Lewis said he had developed a close relationship with the FTX cofounder and added that Bankman-Fried would even come to him for advice.
+The author pointed to Bankman-Fried's maxim that he wanted to do the most possible good — also known as effective altruism.
+"There is still a Sam Bankman-Fried-shaped hole in the world that now needs filling. Like that character would be very useful — with what he wanted to do with the resources," Lewis said.
+That said, Lewis also acknowledged that Bankman-Fried was a "horrible manager."
+Advertisement
+Advertisement
+"If I were a better person, I would have been deeply distressed by all of this. It took about a nanosecond before I thought 'oh my god, this is an incredible story,'" Lewis said.
+Representatives for Lewis did not immediately respond to a request for comment. A representative for Bankman-Fried declined to comment.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2023-10-03 10:37:00</t>
+          <t>2023-10-03 00:00:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>approximated</t>
+          <t>parsed</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['Barbara Kollmeyer']</t>
+          <t>['Grace Kay']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.marketwatch.com/story/the-wild-bunch-have-taken-control-of-the-bond-market-heres-where-they-could-wreak-havoc-next-1448322b</t>
+          <t>https://www.businessinsider.com/sam-bankman-fried-biography-michael-lewis-tom-brady-jail-2023-10</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://news.google.com/rss/articles/CBMihwFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vc3RvcnkvdGhlLXdpbGQtYnVuY2gtaGF2ZS10YWtlbi1jb250cm9sLW9mLXRoZS1ib25kLW1hcmtldC1oZXJlcy13aGVyZS10aGV5LWNvdWxkLXdyZWFrLWhhdm9jLW5leHQtMTQ0ODMyMmLSAYsBaHR0cHM6Ly93d3cubWFya2V0d2F0Y2guY29tL2FtcC9zdG9yeS90aGUtd2lsZC1idW5jaC1oYXZlLXRha2VuLWNvbnRyb2wtb2YtdGhlLWJvbmQtbWFya2V0LWhlcmVzLXdoZXJlLXRoZXktY291bGQtd3JlYWstaGF2b2MtbmV4dC0xNDQ4MzIyYg?oc=5</t>
+          <t>https://news.google.com/rss/articles/CBMiYGh0dHBzOi8vd3d3LmJ1c2luZXNzaW5zaWRlci5jb20vc2FtLWJhbmttYW4tZnJpZWQtYmlvZ3JhcGh5LW1pY2hhZWwtbGV3aXMtdG9tLWJyYWR5LWphaWwtMjAyMy0xMNIBZGh0dHBzOi8vd3d3LmJ1c2luZXNzaW5zaWRlci5jb20vc2FtLWJhbmttYW4tZnJpZWQtYmlvZ3JhcGh5LW1pY2hhZWwtbGV3aXMtdG9tLWJyYWR5LWphaWwtMjAyMy0xMD9hbXA?oc=5</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://www.marketwatch.com</t>
+          <t>https://www.businessinsider.com</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>MarketWatch</t>
+          <t>Business Insider</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Chipotle tests robotic line to make your burrito bowl amid automation push</t>
+          <t>Hong Kong stocks have worst day in three months on worries about rates and real estate</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>More robots are coming to Chipotle (CMG), and one could assemble your burrito bowl in the future.
-On Tuesday, the burrito chain announced it is testing an automated digital assembly line in partnership with Hyphen, a food service platform, to fulfill digital orders.
-On top of the line, an employee will continue to fulfill orders by assembling burritos, tacos, or quesadillas. But underneath, the line will create salads and burrito bowls by positioning bowls under each specified ingredient and portioning them out (with the right amount of salsa so as to not make it too saucy).
-Chipotle is testing an automated makeline for burrito bowls and salads. (Chipotle)
-Chipotle's chief customer and technology officer Curt Garner told Yahoo Finance that as digital sales growth picked up during the pandemic, the team realized it was time to figure out "how to set up the crew members on the digital line to be successful."
-Now, bowls and salads account for 65% of all Chipotle digital orders. Last quarter, digital sales made up 38% of total food and beverage revenue, which came in at $2.5 billion.
-The company began working with Hyphen in 2022, and the burrito bowl invention is part of a larger $50 million dollar venture fund, Cultivate Next, that was introduced in April 2022 to accelerate growth through innovation and technology investments.
-Chipotle's new assembly joins the other robots that the restaurant chain is piloting: Autocado, an avocado processing robot, and Chippy, a robot programmed to make tortilla chips.
-The team is having active discussions on "how many of these technologies are complementary to one another," Garner said, and whether they'll all be at one restaurant or separate. But at the end of the day, Garner emphasized that the crew is crucial to the operation.
-"The best solutions for restaurants and guests are those that have a co-pilot or are co-biotic in nature," he said. "It's about capabilities that improve human experiences."
-Chipotle Mexican Grill announced it is testing an automated digital makeline in collaboration with Hyphen. (Courtesy: Chipotle)
-Still, Chipotle isn't quite ready to fully automate its restaurants. Garner said that the robotic assembly line is still "months away" from being tested in a restaurant.
-Story continues
-When fully rolled out, though, this sort of innovation at a large scale will likely come at a cost to the company.
-"There's certainly a lot of potential for automation in the restaurant space, the issue that you run into is a lot of this equipment is really expensive," Morningstar analyst Sean Dunlop told Yahoo Finance over the phone.
-Dunlop said that may be why we haven't seen Chippy get rolled out yet.
-"For perspective, Chipotle has been working Chippy through its stage gate process for the better part of a couple of years," Dunlop said. "If the return on investment (ROI) were really there and meaningful, we would see this rolled out to corporate stores already like we have with Chipotlane."
-In the background, its fast-casual peer, Sweetgreen (SG) is seeing early success with its first automated production line and restaurant design, dubbed Infinite Kitchen, which has brought in restaurant margins of 26%, significantly higher than any new restaurant opening in its first month at the company.
-Sweetgreen plans to open a second Infinite Kitchen location in Huntington Beach, California, later this year.
-—
-Brooke DiPalma is a reporter for Yahoo Finance. Follow her on Twitter at @BrookeDiPalma or email her at bdipalma@yahoofinance.com.
-Click here for the latest stock market news and in-depth analysis, including events that move stocks
-Read the latest financial and business news from Yahoo Finance</t>
+          <t>Hong Kong CNN —
+Stocks in Hong Kong suffered their worst day in three months on Tuesday on growing concern about China’s weak housing market and persistently high US interest rates.
+The Hang Seng Index ended down 2.7% — its biggest drop since early June — after investors returned from a long holiday weekend. The market benchmark is one of the world’s worst performers this year, having fallen more than 12%, and now stands at its lowest level since November.
+Despite a recent improvement in data, investors remain gripped by worries about China’s economic slowdown, a property market slump, and frictions between Beijing and Washington that have caught tech companies in the crosshairs.
+Real estate stocks were once again among the heaviest losers in Hong Kong.
+Country Garden, one of the country’s largest property developers, sank 4.4%. Its property services arm was down 7.1%. Country Garden has struggled to make debt repayments recently and recorded a huge loss for the first six months. Rival Longfor Properties, a Hang Seng constituent, slid 6.5%.
+Shares of Evergrande, however, closed up 28% after resuming trading following a three-day halt. They have lost 75% since a previous 17-month suspension came to an end in August and now trade like a penny stock.
+Trading in Evergrande New Energy Vehicle, the group’s EV arm, remained suspended, pending the release of an announcement about “inside information,” the firm said in a filing on Tuesday.
+Plunging property sales
+Evergrande Group said last week that its founder and chairman Xu Jiayin had been detained by Chinese authorities on suspicion of crimes, sparking fears that the bankrupt developer could face liquidation. A potential collapse of the firm could put global markets on edge and pile pressure on Beijing to revive the sector.
+New industry data showed China’s 100 biggest developers are still struggling to recover from weak demand.
+Total property sales by the top 100 developers dropped 29% in September from a year ago, marking the fourth straight month of declines, according to data published by Shanghai-based research firm China Real Estate Information Corporation (CRIC) on Saturday. Sales had dropped 35% in August.
+The marginal improvement in September was mainly thanks to Beijing’s support for the property market over the past month, Nomura analysts said in a research report Tuesday.
+“Continued policy relaxation should stabilize property sales, but is not enough to boost stock market sentiment,” they added.
+China has rolled out a series of stimulus measures to boost the country’s ailing property market, including slashing mortgage rates and scrapping restrictions on home buying in Chinese cities.
+Persistently high US rates?
+Market sentiment was also weighed down by concerns that US interest rates could stay elevated after US Treasury yields hit a 16-year high.
+Yields on the 10-year US Treasury, which are considered a proxy for US interest rates, reached 4.7% on Monday, the highest since 2007.
+JPMorgan Chase CEO Jamie Dimon said Monday the Federal Reserve could keeping hiking rates until they hit 7%, a contrarian view but one he has shared twice in as many weeks.
+“This yield surge reflects the market’s response to messaging from the Federal Reserve, indicating the central bank’s commitment to keeping borrowing costs elevated to combat inflation,” said Stephen Innes, managing partner for SPI Asset Management.
+In Asia-Pacific, Japan’s Nikkei 225 dropped 1.6%, and Australia’s S&amp;P/ASX 200 lost 1.3%. Chinese and South Korean markets remained shut for public holidays. European markets were mixed in early trading, while US futures were little changed.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2023-10-03 12:05:30</t>
+          <t>2023-10-03 00:00:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>approximated</t>
+          <t>parsed</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Laura He']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://finance.yahoo.com/news/chipotle-tests-robotic-line-to-make-your-burrito-bowl-amid-automation-push-120530784.html</t>
+          <t>https://www.cnn.com/2023/10/03/investing/global-markets-intl-hnk/index.html</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://news.google.com/rss/articles/CBMieGh0dHBzOi8vZmluYW5jZS55YWhvby5jb20vbmV3cy9jaGlwb3RsZS10ZXN0cy1yb2JvdGljLWxpbmUtdG8tbWFrZS15b3VyLWJ1cnJpdG8tYm93bC1hbWlkLWF1dG9tYXRpb24tcHVzaC0xMjA1MzA3ODQuaHRtbNIBgAFodHRwczovL2ZpbmFuY2UueWFob28uY29tL2FtcGh0bWwvbmV3cy9jaGlwb3RsZS10ZXN0cy1yb2JvdGljLWxpbmUtdG8tbWFrZS15b3VyLWJ1cnJpdG8tYm93bC1hbWlkLWF1dG9tYXRpb24tcHVzaC0xMjA1MzA3ODQuaHRtbA?oc=5</t>
+          <t>https://news.google.com/rss/articles/CBMiS2h0dHBzOi8vd3d3LmNubi5jb20vMjAyMy8xMC8wMy9pbnZlc3RpbmcvZ2xvYmFsLW1hcmtldHMtaW50bC1obmsvaW5kZXguaHRtbNIBT2h0dHBzOi8vYW1wLmNubi5jb20vY25uLzIwMjMvMTAvMDMvaW52ZXN0aW5nL2dsb2JhbC1tYXJrZXRzLWludGwtaG5rL2luZGV4Lmh0bWw?oc=5</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://finance.yahoo.com</t>
+          <t>https://www.cnn.com</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Yahoo Finance</t>
+          <t>CNN</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Powerball drawing: $1.04 billion jackpot winning numbers announced Monday night</t>
+          <t>Winning Powerball numbers for Monday, Oct 2, 2023. Lottery drawing jackpot at $1.20B</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CNN —
-Get your tickets ready: An estimated $1.04 billion dollar jackpot could be yours in Monday night’s Powerball drawing.
-The massive prize is the second-largest jackpot this year and the fourth-largest in the lottery’s history, Powerball said.
-The winning numbers are: 12, 26, 27, 43, 47 and Powerball 5.
-If a player were to pick all the right numbers in Monday’s drawing, they’d have the option of a lump sum payment of $478.2 million – before taxes.
-The jackpot crossed the billion-dollar mark after no ticket matched all six numbers drawn on Saturday: white balls 19, 30, 37, 44 and 46 and red Powerball 22.
-While no one scored the top prize Saturday, there were more than 2.5 million winning tickets at lesser values, including two tickets winning $2 million and five tickets winning $1 million, the lottery announced.
-Overall, your odds of winning a Powerball prize of any amount are 1 in 24.9, the lottery says. But the chances of winning a grand prize are exceedingly slim at 1 in 292.2 million.
-Monday night’s drawing will happen at 10:59 ET. You can watch it on Powerball’s YouTube channel.</t>
+          <t>The Powerball lottery jackpot continues to climb after nobody matched all six numbers on Saturday night and remains in fourth place on the list of top 10 Powerball prizes of all time.
+Grab your tickets and let's see if you're the game's newest millionaire.
+Here are the numbers for the Monday, Oct. 2, Powerball jackpot worth an estimated $1.04 billion with a cash option of $478.2 million.
+Powerball, Mega Millions:Want to win the lottery? Here are luckiest numbers, places to play
+Powerball winning numbers 10/2/23
+The winning numbers for Monday night's drawing were 12, 26, 27, 43, 47, and the Powerball is 5. The Power Play was 2X.
+Did anyone win Powerball last night, Monday, Oct. 2nd, 2023?
+No one matched all six numbers to win the Powerball jackpot.
+Two tickets purchased in Delaware and Michigan matched all five numbers except for the Powerball worth $1 million. Two tickets sold in New York and South Carolina matched all five numbers except for the Powerball and added the Power Play for $2 million.
+Double Play numbers are 11, 26, 35, 40, 43, and the Powerball is 24.
+Nobody matched all six numbers, and zero tickets matched all five numbers except for the Powerball worth $500,000.
+Powerball winner?Lock up your ticket and go hide. What to know if you win the jackpot
+How many lotto numbers in Powerball do you need to win a prize?
+You only need to match one number in Powerball to win a prize. However, that number must be the Powerball worth $4.
+What do I do if I get 2 lottery numbers on Powerball?
+Matching two numbers won't win anything in Powerball unless one of the numbers is the Powerball. A ticket matching one of the five numbers and the Powerball is also worth $4.
+Powerball numbers you need to know:These most commonly drawn numbers could help you win
+When is the next Powerball drawing?
+The Powerball jackpot for Wednesday rose to an estimated $1.20 billion with a cash option of $551.7 million, according to powerball.com.
+Drawings are held three times per week at approximately 10:59 p.m. ET every Monday, Wednesday, and Saturday.
+How to play Powerball
+Mega Millions numbers:Winning Mega Millions numbers for Friday, Sept. 29, 2023. Lottery drawing jackpot at $300M
+Mega Millions lottery drawing
+The Mega Millions jackpot took another leap forward after no one matched all six numbers Friday night. The current Mega Millions jackpot is worth an estimated $300 million, with a cash option of $137.0 million.
+Powerball jackpot winners
+Here is the list of 2023 Powerball jackpot wins, according to powerball.com:
+Results for Top 10 Powerball lottery jackpots
+Here are the all-time top 10 Powerball jackpots, according to powerball.com:
+$2.04 billion — Nov. 7, 2022; California. $1.586 billion — Jan. 13, 2016; California, Florida, Tennessee. $1.20 billion — Oct. 4, 2023; TBA. $1.08 billion — July 19, 2023; California. $768.4 million — Mar. 27, 2019; Wisconsin. $758.7 million — Aug. 23, 2017; Massachusetts. $754.6 million — Feb. 6, 2023; Washington. $731.1 million — Jan. 20, 2021; Maryland. $699.8 million — Oct. 4, 2021; California. $687.8 million — Oct. 27, 2018; Iowa, New York.
+Powerball numbers:Results for Saturday, Sept 30, 2023. Lottery drawing jackpot at $1.04B
+Results for Top 10 U.S. lottery jackpots
+Here are the nation's all-time top 10 Powerball and Mega Millions jackpots, according to powerball.com:
+$2.04 billion, Powerball — Nov. 7, 2022; California. $1.586 billion, Powerball — Jan. 13, 2016; California, Florida, Tennessee. $1.58 million, Mega Millions — Aug. 8, 2023; Florida. $1.537 billion, Mega Millions — Oct. 23, 2018; South Carolina. $1.35 billion, Mega Millions — Jan. 13, 2023; Maine. $1.337 billion, Mega Millions — July 29, 2022; Illinois. $1.20 billion, Powerball — Oct. 4, 2023; TBA. $1.08 billion, Powerball — July 19, 2023; California. $1.05 billion, Mega Millions — Jan. 22, 2021; Michigan. $768.4 million, Powerball — Mar. 27, 2019; Wisconsin.
+Chris Sims is a digital producer at Midwest DOT. Follow him on Twitter: @ChrisFSims.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -730,27 +786,27 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['Kelly Mccleary']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2023/10/02/business/powerball-jackpot-drawing-monday-billion-lottery-trnd/index.html</t>
+          <t>https://www.indystar.com/story/news/2023/10/02/powerball-numbers-october-2-2023-drawing-lottery-jackpot-results-power-ball-lotto-10-2-23/71030872007/</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://news.google.com/rss/articles/CBMiaGh0dHBzOi8vd3d3LmNubi5jb20vMjAyMy8xMC8wMi9idXNpbmVzcy9wb3dlcmJhbGwtamFja3BvdC1kcmF3aW5nLW1vbmRheS1iaWxsaW9uLWxvdHRlcnktdHJuZC9pbmRleC5odG1s0gFsaHR0cHM6Ly9hbXAuY25uLmNvbS9jbm4vMjAyMy8xMC8wMi9idXNpbmVzcy9wb3dlcmJhbGwtamFja3BvdC1kcmF3aW5nLW1vbmRheS1iaWxsaW9uLWxvdHRlcnktdHJuZC9pbmRleC5odG1s?oc=5</t>
+          <t>https://news.google.com/rss/articles/CBMilQFodHRwczovL3d3dy5pbmR5c3Rhci5jb20vc3RvcnkvbmV3cy8yMDIzLzEwLzAyL3Bvd2VyYmFsbC1udW1iZXJzLW9jdG9iZXItMi0yMDIzLWRyYXdpbmctbG90dGVyeS1qYWNrcG90LXJlc3VsdHMtcG93ZXItYmFsbC1sb3R0by0xMC0yLTIzLzcxMDMwODcyMDA3L9IBAA?oc=5</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://www.cnn.com</t>
+          <t>https://www.indystar.com</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>CNN</t>
+          <t>IndyStar</t>
         </is>
       </c>
     </row>
@@ -828,7 +884,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Welcome to the Great Internet Splintering</t>
+          <t>Great news — social media is falling apart</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -847,7 +903,7 @@
 But for all its flaws, I have depended on big platforms. My job as a freelance journalist hinges on a public audience and my ability to keep tabs on developing news. The fatigue I have felt is therefore partly fueled by another, more-pressing concern: Which social network should I bank on? It isn't that I don't want to post; I just don't know where to do it anymore.
 It isn't that I don't want to post; I just don't know where to do it anymore.
 In the past year, I've helplessly migrated alongside most of my network from one new platform to another — Discord, Bluesky, Threads. You name it, I've tried it. The pattern is the same: I sign up for the hot, new app, toy with it for a few days, and then quickly abandon it. While widespread platform migrations have taken place successfully over the years — I migrated from Google's Orkut, a popular platform in India and Brazil in the late aughts, to Facebook to Instagram to TikTok — I have never before found myself in no man's land. If none of these platforms are lining up to be the new Facebook, what is the future?
-Chand Rajendra-Nicolucci, who researches digital public infrastructure at the University of Michigan, said there's a reboot taking place now and that social media's future might be "more private and more fragmented." In a white paper published earlier this year, he and his colleagues envisioned a "pluriverse" consisting of existing platforms and an ecosystem of "very small online platforms" — private communities and niche services that host the kind of intimate or interest-specific conversations poorly served by today's digital public sphere.
+Chand Rajendra-Nicolucci, who researches digital public infrastructure at the University of Massachusetts Amherst, said there's a reboot taking place now and that social media's future might be "more private and more fragmented." In a white paper published earlier this year, he and his colleagues envisioned a "pluriverse" consisting of existing platforms and an ecosystem of "very small online platforms" — private communities and niche services that host the kind of intimate or interest-specific conversations poorly served by today's digital public sphere.
 Advertisement
 Advertisement
 In a way, the pluriverse is already here. People can be active on half a dozen social-media apps, using each for a unique purpose and audience. On "public" platforms such as LinkedIn and X, formerly Twitter, I carefully curate my presence and use them exclusively as public-broadcasting tools for promotions and outreach. But for socializing, I retreat to various tight-knit, private groups such as iMessage threads and Instagram's Close Friends list, where I can be more spontaneous and personal in what I say. But while this setup is working OK for now, it's a patchwork solution.
@@ -866,7 +922,7 @@
 At its best, Steve Teixeira, the chief product officer at Mozilla, said that social media facilitated connection, regardless of geographic or temporal boundaries, and helps people stay informed, encounter novel ideas, and access vital services. At the moment, though, "it isn't doing any of these things particularly well," he said. The problem is that social media is trying to do too many things at once. Splintered social media would let each of the internet's key functions thrive in its own context — you could stay in touch with family members and keep up with your political representatives without your private memories getting wedged in between political drama.
 Instead of living in Facebook city under Facebook's laws, the decentralized approach offers everyone more control over the social-media experience.
 The other problem is that users have very little control over what they experience online. Studies have found that news overload from social media can cause stress, anxiety, fatigue, and lack of sleep. By democratizing social media, users can turn those negative health effects around by taking more control over who they're associated with, what they look at in their feeds, and how algorithms are influencing their social experience. And by splintering our time across a variety of platforms — each with a different approach to content moderation — the online communication ecosystem ends up better reflecting the diversity of the people who use it. People who wish to keep their data to themselves can live inside tight-knit circles. Those who don't want a round-the-clock avalanche of polarizing content can change what their feed shows them. Activists looking to spread a message can still reach millions. The list goes on.
-"Instead of policymakers and users having to plead, poke, and prod platforms to change," Rajendra-Nicolucci said, "decentralization would enable them to take matters into their own hands, allowing many different answers to the question: 'How should platform X work to coexist?'"
+"Instead of policymakers and users having to plead, poke, and prod platforms to change," Rajendra-Nicolucci said, "decentralization would enable them to take matters into their own hands, allowing many different answers to the question: 'How should platform X work?' to coexist."
 Tailoring social media to people's needs could revolutionize how we spend time online. Swapping out virality-incentivized algorithms in favor of ones that resonate with diverse audiences, for example, can reduce bias and polarization. And experts have found that a collection of networks would "optimize itself solely for public good," rather than fall into the pitfalls of traditional platforms — an unhealthy obsession with metrics and meaningless interactions.
 It's hard to predict the future, least of all when it comes to online services where new apps can go viral — and then fail — in a flash, but the breakup of monolithic social-media platforms and the rise of myriad new social experiences has felt like an urgent, long-overdue turn of events. It has propelled millions, including me, to question the status quo — did I need to add a dozen hashtags in hopes of making my sunset picture go viral? — and embrace a healthier relationship with social media. No one knows what the next major social platform will look like. But until it emerges, I expect to continue living a splintered and nomadic online social life.
 Shubham Agarwal is a freelance technology journalist from Ahmedabad, India whose work has appeared in Wired, The Verge, Fast Company, and more.</t>
@@ -911,375 +967,520 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Are you a robot?</t>
+          <t>Chipotle tests automation for burrito bowls and salads</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Why did this happen?
-Please make sure your browser supports JavaScript and cookies and that you are not blocking them from loading. For more information you can review our Terms of Service and Cookie Policy.</t>
+          <t>Chipotle Mexican Grill is testing whether automation can make customers' burrito bowls and salads.
+It's the second time the burrito chain has publicly announced testing automation at its innovation center. Chippy, Chipotle's first foray into automation, is a robot that makes tortilla chips. The company began testing Chippy at a California restaurant a year ago after it passed the first round of testing.
+Restaurants ranging from Sweetgreen to Starbucks have been investing in automation to cut down on labor costs and improve order consistency and speed. But robotics and artificial intelligence software can be expensive, so it will likely be years before the technology pays off for restaurants.
+Still, many operators have big hopes for automation's future in the restaurant industry. Sweetgreen opened its first automated location in May and CEO Jonathan Neman already expects all of the chain's future restaurants to be automated in five years.
+The Chipotle test announced Tuesday is part of a collaboration with Hyphen, a startup that's trying to automate restaurant kitchens. Last year, Chipotle invested an undisclosed amount in Hyphen, formerly known as Ono Food. The startup has a valuation of $104 million, according to PitchBook.
+All Chipotle restaurants have two make lines to assemble orders: one in the front for diners who order in person and another in the kitchen for digital orders. Roughly two-thirds of all Chipotle digital orders are either burrito bowls or salads, according to Chipotle.
+The Hyphen robot will make burrito bowls and salads for digital orders only. The technology moves the bowls underneath the digital make line to dispense the correct ingredients. Simultaneously, an employee can assemble digital orders for other items, such as tacos, quesadillas and burritos, on the digital make line. When the robot is done making an order, it sends the bowl or salad back up to the surface so employees can properly package the order.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2023-10-03 02:48:45</t>
+          <t>2023-10-03 00:00:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>approximated</t>
+          <t>parsed</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>['Amelia Lucas']</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.cnbc.com/2023/10/03/chipotle-tests-automation-for-burrito-bowls-and-salads-.html</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://news.google.com/rss/articles/CBMib2h0dHBzOi8vd3d3LmJsb29tYmVyZy5jb20vbmV3cy9hcnRpY2xlcy8yMDIzLTEwLTAzL3Rlc2xhLXNhbGVzLWRyb3Atc2Vlcy1ieWQtY2xvc2UtZ2FwLWluLXJhY2UtZm9yLWV2LXN1cHJlbWFjedIBAA?oc=5</t>
+          <t>https://news.google.com/rss/articles/CBMiXGh0dHBzOi8vd3d3LmNuYmMuY29tLzIwMjMvMTAvMDMvY2hpcG90bGUtdGVzdHMtYXV0b21hdGlvbi1mb3ItYnVycml0by1ib3dscy1hbmQtc2FsYWRzLS5odG1s0gEA?oc=5</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.bloomberg.com</t>
+          <t>https://www.cnbc.com</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Bloomberg</t>
+          <t>CNBC</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GM lays off 164 more workers due to UAW strike</t>
+          <t>Rouble recovers after slide past 100 vs dollar to 7-week low</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>General Motors has laid off more employees as a result of the United Auto Workers union's strike, bringing the company's total tally of workers furloughed in connection with the work stoppage above 2,100.
-The UAW is waging a simultaneous yet limited strike against all Detroit's Big Three automakers, but GM is the only company that has not been spared so far in the union's incremental strike escalations.
-Ticker Security Last Change Change % GM GENERAL MOTORS CO. 32.47 -0.50 -1.52%
-General Motors Co.
-The union's strike began on Sept. 15, starting with a Ford plant in Michigan, a GM plant in Wentzville, Missouri, and a Stellantis plant in Ohio. Then on Sept. 22, the UAW targeted 38 parts distribution facilities for GM and Stellantis. In the third round on Friday, workers at GM's assembly plant in Lansing, Michigan, and Ford's assembly plant in Chicago walked off the job.
-Hours later, GM said it would be forced to furlough 130 workers at its Parma, Ohio, metal center and 34 from its Marion, Indiana, metal center.
-UAW STRIKE AGAINST FORD, GM, STELLANTIS COST US ECONOMY NEARLY $4B SO FAR
-"The UAW leadership’s decision to call a strike at GM Wentzville Assembly, and now GM Lansing Delta Township Assembly, continues to have negative ripple effects," the company said in a statement. "Beginning Monday, October 2nd, a portion of GM’s Parma Metal Center and Marion Metal Center represented workforce will have no work available. The affected team members are not expected to return until the strike has been resolved."
-"We have said repeatedly that nobody wins in a strike, and this is yet another demonstration of that fact," the statement continued. "We will continue to bargain in good faith with the union to reach an agreement as quickly as possible."
-AFTER VISITING STRIKE, BIDEN WILL LEAVE NEGOTIATIONS ‘UP TO THE UAW LEADERSHIP,’ WHITE HOUSE SAYS
-GM previously laid off around 2,000 workers following the first strike round, saying the strike at its Wentzville facility had forced it to shut down its Fairfax, Kansas, plant due to a parts shortage.
-Last month, Stellantis laid off roughly 370 workers as a result of the strike, and Ford temporarily furloughed 600, according to Forbes.
-Ticker Security Last Change Change % STLA STELLANTIS NV 18.91 -0.22 -1.15% F FORD MOTOR CO. 12.31 -0.11 -0.89%
-GET FOX BUSINESS ON THE GO BY CLICKING HERE
-Ford executives warned Friday in a media briefing that a prolonged work stoppage at its assembly plants would not only hurt the company, but could lead to as many as 500,000 workers at suppliers being laid off.
-Reuters contributed to this report.</t>
+          <t>A view shows a Russian one rouble coin in front of a screen displaying the Spasskaya tower of the Moscow Kremlin in this illustration picture taken August 22, 2023. REUTERS/Maxim Shemetov/Illustration/File photo Acquire Licensing Rights
+Summary Rouble falls past 100 vs dollar in early trade
+Russian currency recovers some ground during session
+Crossing 100 threshold in Aug led to rate hike
+Kremlin: No need for concern over rouble rate
+Oct 3 (Reuters) - The Kremlin on Tuesday stressed that there was no need for concern after the Russian rouble weakened past the symbolic threshold of 100 to the dollar in early trade before recovering slightly, weighed down by foreign currency outflows.
+The rouble's last tumble into triple digits in August led the Bank of Russia to make an emergency 350-basis-point rate hike to 12% and authorities discussed reintroducing controls to buttress the currency.
+By 1150 GMT, the rouble was 0.6% stronger against the dollar at 99.17, having hit 100.2550 in early trade, a more than seven-week low.
+It had gained 1% to trade at 104.91 versus the euro and firmed 0.5% against the yuan to 13.53 .
+"There is still no cause for concern," Kremlin spokesman Dmitry Peskov told reporters. "Macroeconomic stability is fully ensured by the actions of the macro regulator and the government, so there are no grounds for concern here."
+Brent crude oil , a global benchmark for Russia's main export, was down 0.8% at $90.01 a barrel, its weakest in almost a month, but still well above its 2023 average.
+The Russian currency tends to come under pressure at the start of each month, after losing the support of a favourable month-end tax period that usually sees exporters convert FX revenues to meet local liabilities.
+"Expensive oil and an increase in the key rate are improving the outlook for the rouble, but in the medium-term," Promsvyazbank analysts said. They expected the rouble to make a short-lived move beyond 100 to the dollar in the absence of new support measures from the authorities.
+'PSYCHOLOGICAL BARRIER'
+President Vladimir Putin's economic adviser rebuked the central bank as the rouble slid to 101.75 per dollar in August, blaming its loose policy in a sign of growing internal discord.
+"This level (100) is not a technical resistance, it's an important psychological barrier," said Alor Broker's Alexei Antonov. "For now, everything speaks in favour of the rouble continuing to get cheaper."
+Following the August emergency hike, the central bank raised rates again in September to 13%. Analysts polled by Reuters expect the central bank, also grappling with stubborn inflationary pressure, to tighten monetary policy again at its next scheduled meeting on Oct. 27.
+The rouble has charted a turbulent course since Russia invaded Ukraine in February 2022, slumping to a record low of 120 against the dollar in March last year before recovering to a more than seven-year high a few months later, supported by capital controls and surging export revenue.
+Falling exports, hit by Western sanctions and shifting trade flows, combined with a recovery in imports this year has caused the rouble to weaken. Russia's current account surplus shrank 86% year-on-year to $25.6 billion in January-August.
+Reporting by Lidia Kelly in Melbourne and Alexander Marrow in London; Editing by Andrew Heavens and Alison Williams
+Our Standards: The Thomson Reuters Trust Principles.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2023-10-02 18:43:17</t>
+          <t>2023-10-03 00:00:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>approximated</t>
+          <t>parsed</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>['Breck Dumas']</t>
+          <t>['Alexander Marrow', 'Thomson Reuters', "Moscow-Based Reporter Covering Russia'S Economy", 'Markets', "The Country'S Financial", 'Retail', 'Technology Sectors', 'With A Particular Focus On The Western Corporate Exodus Russia', 'The Domestic Players Eyeing Opportunities As The Dust Settles. Before Joining Reuters', "Alexander Worked On Sky Sports News' Coverage Of The Olympics In Brazil"]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.foxbusiness.com/economy/gm-lays-off-164-workers-uaw-strike</t>
+          <t>https://www.reuters.com/markets/currencies/russian-rouble-weakens-past-100-vs-dollar-2023-10-03/</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://news.google.com/rss/articles/CBMiRmh0dHBzOi8vd3d3LmZveGJ1c2luZXNzLmNvbS9lY29ub215L2dtLWxheXMtb2ZmLTE2NC13b3JrZXJzLXVhdy1zdHJpa2XSAUpodHRwczovL3d3dy5mb3hidXNpbmVzcy5jb20vZWNvbm9teS9nbS1sYXlzLW9mZi0xNjQtd29ya2Vycy11YXctc3RyaWtlLmFtcA?oc=5</t>
+          <t>https://news.google.com/rss/articles/CBMiYGh0dHBzOi8vd3d3LnJldXRlcnMuY29tL21hcmtldHMvY3VycmVuY2llcy9ydXNzaWFuLXJvdWJsZS13ZWFrZW5zLXBhc3QtMTAwLXZzLWRvbGxhci0yMDIzLTEwLTAzL9IBAA?oc=5</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.foxbusiness.com</t>
+          <t>https://www.reuters.com</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Fox Business</t>
+          <t>Reuters</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dow futures fall 100 points as Treasury yields jump to multiyear highs: Live updates</t>
+          <t>Strong U.S. dollar, rising Treasury yields keep bulls on sidelines</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>(Kitco News) - Gold and silver prices are lower again Tuesday morning, with December gold futures hitting another 10-month low and December silver futures another 6.5-month low. A still-strong U.S. dollar and rising U.S. Treasury yields that are at 16-year highs are keeping both precious metals in a tailspin. December gold was last down $6.50 at $1,840.80 and December silver was down $0.216 at $21.21.
+The marketplace is still digesting the “higher for longer” U.S. interest rate scenario. The benchmark 10-year Treasury note yield is at its highest level since 2007. A Barron’s headline today reads: “The bond sell off is gathering pace. Why the Fed isn’t intervening.” The story suggests the Federal Reserve is content with rising Treasury yields as it helps in the inflation battle the central bank is presently waging.
+Asian and European stocks were mostly lower overnight. U.S. stock indexes are pointed to slightly higher openings when the New York day session begins.
+In overnight news, Australia’s central bank left its main interest rate unchanged, but said further monetary policy tightening may be warranted.
+The key outside markets today see the U.S. dollar index higher and hitting another 10-month high. Nymex crude oil prices are a bit weaker and trading around $88.50 a barrel. Meantime, the benchmark U.S. Treasury 10-year note yield is presently fetching 4.699% and this week has hit a 16-year high. December Comex gold futures hit a 10-month low overnight, while silver hit a 6.5-month low.
+U.S. economic data due for release Tuesday includes the weekly Johnson Redbook retail sales report, the IDB/TIPP economic optimism index and domestic auto industry sales.
+Technically, the gold futures bears have the solid overall near-term technical advantage. Prices are in an accelerating four-month-old downtrend on the daily bar chart. Bulls’ next upside price objective is to produce a close in December futures above solid resistance at $1,900.00. Bears' next near-term downside price objective is pushing futures prices below solid technical support at $1,800.00. First resistance is seen at the overnight high of $1,845.30 and then at $1,850.00. First support is seen at the overnight low of $1,830.90 and then at $1,825.00. Wyckoff's Market Rating: 1.0
+The silver bears have the solid overall near-term technical advantage. Silver bulls' next upside price objective is closing December futures prices above solid technical resistance at $23.00. The next downside price objective for the bears is closing prices below solid support at $20.00. First resistance is seen at $21.50 and then at $22.00. Next support is seen at $21.00 and then at the overnight low of $20.87. Wyckoff's Market Rating: 2.0.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2023-10-03 00:00:00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>parsed</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>['Http', 'Www.Facebook.Com Kitconews']</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.kitco.com/news/2023-10-03/Strong-U-S-dollar-rising-Treasury-yields-keep-bulls-on-sidelines.html</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://news.google.com/rss/articles/CBMia2h0dHBzOi8vd3d3LmtpdGNvLmNvbS9uZXdzLzIwMjMtMTAtMDMvU3Ryb25nLVUtUy1kb2xsYXItcmlzaW5nLVRyZWFzdXJ5LXlpZWxkcy1rZWVwLWJ1bGxzLW9uLXNpZGVsaW5lcy5odG1s0gEA?oc=5</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>https://www.kitco.com</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Kitco NEWS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Tesla reported 435,059 deliveries for the third quarter, and production of 430,488 vehicles</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Tesla vehicles waiting to be loaded on board a cargo vessel at Nangang port, in Shanghai, China, on Sept. 6, 2023.
+Tesla posted its third-quarter vehicle production and delivery report for 2023 on Monday.
+Here are the key numbers from the electric vehicle maker:
+Total deliveries Q3 2023: 435,059
+Total production Q3 2023: 430,488
+During the previous quarter, Tesla reported total deliveries of 466,140 and total vehicle production of 479,700. During the same period in 2022 Tesla reported total vehicle production of 365,923 and deliveries of 343,830.
+"A sequential decline in volumes was caused by planned downtimes for factory upgrades, as discussed on the most recent earnings call," the company said. "Our 2023 volume target of around 1.8 million vehicles remains unchanged."
+Despite its report of a nearly 7% decline in vehicle deliveries compared to the previous quarter, shares of Tesla closed nearly flat for the day at $251.60 on Monday.
+On its last earnings call in July, CEO Elon Musk cautioned that Tesla would "continue to target 1.8 million vehicle deliveries this year" but expected third-quarter production to decline slightly following "summer shutdowns for a lot of factory upgrades."
+The company is still not reporting on production or delivery numbers for the Semi, a class 8 electric truck, though it delivered some to an early customer, PepsiCo, which is using the fully electric trucks for some deliveries.
+Wall Street was expecting Tesla deliveries to reach 461,640 for the period ending Sept. 30, according to a consensus of analysts polled by StreetAccount. An independent Tesla researcher, who uses the handle Troy Teslike on social media, was expecting deliveries of 441,000 vehicles.
+Tesla's head of investor relations, Martin Viecha, sent out a company-compiled consensus to select investors, some of whom shared it publicly on social media. That number showed Wall Street was expecting around 455,000 total deliveries, with a median estimate of 453,128 deliveries for the quarter, based on 25 analysts' estimates.
+Tesla groups its deliveries into two categories, Model S and X vehicles, and Model 3 and Y vehicles, but doesn't report individual model or region-specific numbers. Deliveries are the closest approximation to vehicles sold reported by the company.
+Tesla slashed prices throughout the third quarter on its inventory vehicles and existing models, which put pressure on competitors to follow suit.
+Tesla also revealed a revamped version of its Model 3 sedan, dubbed the "Highland," with both new exterior and interior features, and started selling it in some regions outside the U.S. The interior for the refreshed Model 3 includes touchscreen displays for rear-seat passengers and ventilated seats, among other items. The vehicle is sold with a long-range battery option that gets about 390 miles, or 629 km, per charge.
+In August, Zachary Kirkhorn announced he was stepping aside as CFO, and the company said Chief Accounting Officer Vaibhav Taneja would now serve both roles. Tesla's next earnings call will be the first with Taneja in the CFO seat.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2023-10-02 00:00:00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>parsed</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>['Lora Kolodny']</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://www.cnbc.com/2023/10/02/tesla-tsla-q3-2023-vehicle-delivery-and-production-numbers.html</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>https://news.google.com/rss/articles/CBMiX2h0dHBzOi8vd3d3LmNuYmMuY29tLzIwMjMvMTAvMDIvdGVzbGEtdHNsYS1xMy0yMDIzLXZlaGljbGUtZGVsaXZlcnktYW5kLXByb2R1Y3Rpb24tbnVtYmVycy5odG1s0gFjaHR0cHM6Ly93d3cuY25iYy5jb20vYW1wLzIwMjMvMTAvMDIvdGVzbGEtdHNsYS1xMy0yMDIzLXZlaGljbGUtZGVsaXZlcnktYW5kLXByb2R1Y3Rpb24tbnVtYmVycy5odG1s?oc=5</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>https://www.cnbc.com</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>CNBC</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Ford, GM Lay Off About 500 Factory Workers as UAW Strike Effects Ripple Out</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>This copy is for your personal, non-commercial use only. Distribution and use of this material are governed by our Subscriber Agreement and by copyright law. For non-personal use or to order multiple copies, please contact Dow Jones Reprints at 1-800-843-0008 or visit www.djreprints.com.
+https://www.wsj.com/business/autos/ford-gm-lay-off-about-500-factory-workers-as-uaw-strike-effects-ripple-out-15bf8fba</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2023-10-03 07:29:00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>approximated</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>['Mike Colias']</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://www.wsj.com/business/autos/ford-gm-lay-off-about-500-factory-workers-as-uaw-strike-effects-ripple-out-15bf8fba</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>https://news.google.com/rss/articles/CBMidmh0dHBzOi8vd3d3Lndzai5jb20vYnVzaW5lc3MvYXV0b3MvZm9yZC1nbS1sYXktb2ZmLWFib3V0LTUwMC1mYWN0b3J5LXdvcmtlcnMtYXMtdWF3LXN0cmlrZS1lZmZlY3RzLXJpcHBsZS1vdXQtMTViZjhmYmHSAQA?oc=5</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>https://www.wsj.com</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>The Wall Street Journal</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>A woman was found trapped under a driverless car. It’s not what it looks like, the car company said</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>CNN —
+A pedestrian in downtown San Francisco was found critically injured and trapped underneath a driverless car Monday night. But the company that operates the autonomous car says it’s not at fault.
+San Francisco Fire Department spokesperson Justin Schorr told CNN early Tuesday that the victim has multiple life-threatening injuries.
+The driverless vehicle was operated by Cruise, a San Francisco-based self-driving car company and subsidiary of General Motors (GM). But the company says another vehicle was to blame for the pedestrian’s injury.
+“A human-driven vehicle struck a pedestrian while traveling in the lane immediately to the left of a Cruise AV,” said Cruise spokesperson Navideh Forghani in a statement to CNN. “The initial impact was severe and launched the pedestrian directly in front of the AV. The AV then braked aggressively to minimize the impact.” Forghani says the driver of the other vehicle fled the scene.
+Schorr said representatives of the company responded to the scene of the accident “very swiftly” and have been cooperating with investigators.
+“There was no driver and no passenger in the car to be able to tell us what happened,” Schorr said. But he added that Cruise cars have their own cameras and collect a variety of telemetric data which may help in the investigation of the accident. “It’s a very unique type of response for San Francisco,” he said.
+The pedestrian, who has not been named, is being treated at San Francisco General Hospital for what a Fire Department spokesperson described as “multiple life-threatening injuries.” The San Francisco Police Department is investigating the accident, but has not yet commented on the cause.
+“Our heartfelt concern and focus is the wellbeing of the person who was injured and we are actively working with police to help identify the responsible driver,” the Cruise spokesperson said.
+Controversial driverless cars
+Cruise has been the subject of controversy in San Francisco after California regulators last month approved robotaxi companies to operate their driverless cars 24/7 throughout the city.
+The company’s self-driving cars have been blamed for massive traffic jams and multiple collisions, including one that involved a fire truck. One of its driverless taxis drove into a construction area and stopped in wet concrete.
+Cruise agreed to the California DMV’s request to reduce its fleet by 50% while it takes corrective action.
+The recent events underscore the challenges of creating safe, fully driverless passenger vehicles.
+General Motors acquired Cruise Automation in 2016 for $1 billion, solidifying its place in the autonomous vehicles race, but many companies have since scaled back, or abandoned their driverless car ambitions. The endeavor has proven costly, and mastering all situations that humans might face behind the wheel is difficult and time-consuming.
+Ridesharing giants Uber and Lyft have both sold autonomous vehicle units in recent years. Even Tesla CEO Elon Musk, who has been optimistic about autonomous vehicle technology, has yet to fully deliver on his promise.
+But advocates say driverless cars remain safer than human-operated vehicles.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2023-10-03 00:00:00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>parsed</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>['Andy Rose']</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://www.cnn.com/2023/10/03/tech/driverless-car-pedestrian-injury/index.html</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>https://news.google.com/rss/articles/CBMiT2h0dHBzOi8vd3d3LmNubi5jb20vMjAyMy8xMC8wMy90ZWNoL2RyaXZlcmxlc3MtY2FyLXBlZGVzdHJpYW4taW5qdXJ5L2luZGV4Lmh0bWzSAVNodHRwczovL2FtcC5jbm4uY29tL2Nubi8yMDIzLzEwLzAzL3RlY2gvZHJpdmVybGVzcy1jYXItcGVkZXN0cmlhbi1pbmp1cnkvaW5kZXguaHRtbA?oc=5</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>https://www.cnn.com</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>CNN</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Stocks fall as Treasury yields jump to multiyear highs: Live updates</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>Traders on the floor of the New York Stock Exchange.
-Stock futures turned down on Tuesday as traders kept an eye on rising Treasury yields, which hit a 16-year high.
-Dow Jones Industrial Average futures declined 167 points, or 0.5%. Futures tied to the S&amp;P 500 dropped 0.7%, while Nasdaq 100 futures fell 0.8%.
-The 10-year Treasury yield traded at 4.735%, climbing to its highest level since Aug. 15, 2007. The benchmark yield has surged in the past month, as traders assess the possibility of tighter Federal Reserve for longer.
+Stocks fell Tuesday as traders kept an eye on rising Treasury yields, which hit a 16-year high.
+The Dow Jones Industrial Average lost 162 points, or 0.5%. The S&amp;P 500 slid 0.6%, and the Nasdaq Composite pulled back 0.8%.
+Seasoning and spice manufacturer McCormick &amp; Company led the broad market index's losses on Tuesday, falling more than 7% after announcing its quarterly earnings. Kellogg also declined by 7%, followed by Veralto and Airbnb down 4.1% and 3.4%, respectively.
+The 10-year Treasury yield last traded at 4.704%, easing from 4.745% earlier Tuesday morning, which was its highest level since Aug. 15, 2007. The benchmark yield has surged in the past month, as traders assess the possibility of tighter Federal Reserve for longer.
 Investors have been fretting recently over the potential of higher interest Federal Reserve for longer, fearing that tighter monetary policy could tip the economy into a recession. This has pushed Treasury yields to levels not seen in more than a decade.
 "Stocks are attempting to rebound but bulls remain chastened and diffident, with little appetite to chase on the upside," wrote Adam Crisafulli of Vital Knowledge. "At this point, buyers seem willing to miss the next ~2-4% of an advance to ensure the lift is on more stable footing before participating."
-Wall Street is coming off a mixed session, after lawmakers in Washington arrived at a short-term agreement over the weekend that headed off a government shutdown. The 30-stock Dow closed lower by 0.2%, while the S&amp;P 500 closed marginally higher. The Nasdaq Composite rose for a fourth day in a row.
+Wall Street is coming off a mixed session, after lawmakers in Washington arrived at a short-term agreement over the weekend that headed off a government shutdown.
 Investors are hoping to turn the page on a disappointing September for stocks. All three major indexes closed the month and the third quarter lower. The S&amp;P 500 alone lost nearly 5% in September.
 That means key economic reports — such as last month's payroll reports, due Friday — and the kick off of earnings reporting season next week are back in focus.
-"Investors expect a solid upcoming earnings season, but we believe expectations are too optimistic for the balance of 2023 and 2024," said Richard Saperstein, chief investment officer at Treasury Partners.
-"The most immediate risk to stocks is if companies are meaningfully affected by the economic slowing that is occurring from higher interest rates, which is a prominent risk that the market is ignoring right now," he added.
 On the economic data front, investors will be watching the Job Openings and Labor Turnover Survey for August, due Tuesday morning. Economists polled by Dow Jones anticipate 8.8 million job openings.</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>2023-10-02 00:00:00</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>parsed</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>['Hakyung Kim Brian Evans', 'Hakyung Kim', 'Brian Evans']</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>https://www.cnbc.com/2023/10/02/stock-market-today-live-updates.html</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>https://news.google.com/rss/articles/CBMiRGh0dHBzOi8vd3d3LmNuYmMuY29tLzIwMjMvMTAvMDIvc3RvY2stbWFya2V0LXRvZGF5LWxpdmUtdXBkYXRlcy5odG1s0gFIaHR0cHM6Ly93d3cuY25iYy5jb20vYW1wLzIwMjMvMTAvMDIvc3RvY2stbWFya2V0LXRvZGF5LWxpdmUtdXBkYXRlcy5odG1s?oc=5</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>https://www.cnbc.com</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>CNBC</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Award-winning technical strategist Tom DeMark says S&amp;P 500 will see countertrend rally</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Tom DeMark, the award-winning technical strategist, says the stock market is due for a countertrend rally that will soon exhaust itself.
-DeMark, who has advised investors including Paul Tudor Jones and Steven A. Cohen, told MarketWatch that last week, various major indexes recorded bottoms.
-“Into their lows Wednesday, various market indices recorded daily 13 bottoms which served to offset the daily 13 tops recorded at their July highs. Consequently, stock indices are expected to retrace a portion of their prior two month decline,” said DeMark, the founder and chief executive of DeMark Analytics. See DeMark’s analysis on his website Symbolik.
-He focuses on the number of days — which don’t have to be consecutive — that there was a close lower than the low of two days ago. Subject to various conditions, when the countdown reaches 13, a buy signal is triggered. (The opposite is the case on the way up.)
-He said there were two equal percentage declines from the July peak to last week’s low, of about 6%, so there should be a 62% replacement of the entire decline.
-“This would translate into [S&amp;P 500] upside projection of 4,466. Other timing measures arrive at comparable upside levels,” he said. DeMark said the expected duration should be three to four weeks. The S&amp;P 500 SPX ended fractionally higher at 4,288.39 on Monday, but is down 7% from its July 31 peak.
-He says the daily S&amp;P 500 charge shows the index topped on Sept. 1, when its secondary high traded slightly above what he called the magnet price, which was the close on July 27, DeMark said. The low last Tuesday was the S&amp;P 500’s trend channel lower band, he added.
-DeMark said markets top not because of smart sellers but rather when the last buyer has bought, and vice versa. That means, markets rarely bottom on good news or rarely top on bad news.
-He added that at times, markets are on the threshold of recording meaningful tops and bottoms, but if the required conditions aren’t met, the opportunity is lost and the process must then reset. That occurred in May, when he said the Nasdaq was on the verge of exhaustion, but then associated conditions were not met. In July, by contrast, all the conditions required for a market top were present.</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2023-10-03 10:44:00</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>approximated</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>['Steve Goldstein']</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>https://www.marketwatch.com/story/award-winning-technical-strategist-tom-demark-says-s-p-500-will-see-countertrend-rally-4a713d7</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>https://news.google.com/rss/articles/CBMigAFodHRwczovL3d3dy5tYXJrZXR3YXRjaC5jb20vc3RvcnkvYXdhcmQtd2lubmluZy10ZWNobmljYWwtc3RyYXRlZ2lzdC10b20tZGVtYXJrLXNheXMtcy1wLTUwMC13aWxsLXNlZS1jb3VudGVydHJlbmQtcmFsbHktNGE3MTNkN9IBAA?oc=5</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>https://www.marketwatch.com</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>MarketWatch</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Gold bulls can look forward to a bright future despite headwinds - Heraeus</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Get all the essential market news and expert opinions in one place with our daily newsletter. Receive a comprehensive recap of the day's top stories directly to your inbox. Sign up here!
-(Kitco News) - Even as markets watch gold prices fall into the low 1830s as the fourth quarter gets underway, interest rate history favors gold bugs in the medium and long term, according to the latest precious metals report from Heraeus.
-âThe gold price tends to rise following the first cut of US interest rate cycles,â the analysts write. âOn average since 1984, one calendar year after the Federal Reserve first cuts its rate after a hiking cycle, gold is 10% higher than the day of the decision to reduce interest rates, and after two years is 18% higher. The dollar tends to weaken, yields on U.S. Treasuries fall, and the economy tends to have deteriorated. All of these elements can act as a tailwind for the gold price.â
-The analysts say that after the yield on the 10-year treasury note peaks, itâs only a matter of time before Fed Chair Jerome Powell begins to cut. âThe last rate hike of the cycle also tends to coincide with the peak in the yield on 10-year U.S. Treasuries,â they write. âSince 1984, interest rate cuts have never lagged the peak in 10-year U.S. Treasury notes by more than one year and seven months â this being the outlier in 1989. Excluding 1989, cuts have followed the peak by an average of ~10 months.â
-They note, however, that this does not constitute a guarantee. âTwo years after the first interest rate reduction in 1995, gold was 16% lower at $325.50/oz,â they say. âOn the other hand, goldâs relative performance to the upside following interest rate cuts has grown since the 2001 cycle.â
-U.S. government bond yields are now at the highest rate in 16 years, hitting a fresh high of 4.7% just after noon EDT on Monday. âThe yield on longdated US Government debt has not hit 4.5% since September 2007, the month that interest rates were lowered 50 bp from 5.25% to 4.75% and the US was on the brink of recession,â note the Heraeus analysts. âThis suggests the higher-for-longer message from the Fed may now be sinking in for investors, and raises the expectation that for this cycle there could be a more prolonged period before interest rates begin to fall.â
-They acknowledge that goldâs short-term outlook is challenged by the surge in yields. âThe average rate tightening cycle has lasted for 21 months with a total Federal Funds increase of 3.02%, but this point is clearly past,â the analysts write. âHistorically, long-term yields peak shortly before the Fed stops increasing short-term rates. Inflation may continue to climb well after the Fed curtails rate hikes. The uptick in consumer prices in August highlights that despite a Fed pause in September, inflation may not be tamed just yet, and that gold is likely to face headwinds until at least the new year or until yields flag.â
-Another key headwind for the yellow metal is the strength of the U.S. dollar, which continues to outperform, with DXY flirting with 107 on Monday afternoon, a level it has not breached since Nov. 22. âThe strength in the U.S. dollar in the last week may be a sign that traders are beginning to accept that interest rates may be higher for longer,â they write, noting that the dollar index âis up ~7% since mid-July, against other major currencies.â
-The Heraeus analysts believe the next significant technical support for gold is all the way down at $1,800 per ounce, a price the precious metal has not seen since the days before Christmas last year.</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2023-10-02 00:00:00</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>parsed</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>['Http', 'Www.Facebook.Com Kitconews']</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>https://www.kitco.com/news/2023-10-02/Gold-bulls-can-look-forward-to-a-bright-future-despite-headwinds-Heraeus.html</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>https://news.google.com/rss/articles/CBMic2h0dHBzOi8vd3d3LmtpdGNvLmNvbS9uZXdzLzIwMjMtMTAtMDIvR29sZC1idWxscy1jYW4tbG9vay1mb3J3YXJkLXRvLWEtYnJpZ2h0LWZ1dHVyZS1kZXNwaXRlLWhlYWR3aW5kcy1IZXJhZXVzLmh0bWzSAQA?oc=5</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>https://www.kitco.com</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Kitco NEWS</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Abercrombie &amp; Fitch launches investigation into ex-CEO sexual misconduct claims</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>The largest event described to the BBC was hosted in a private villa at a five-star hotel in 2011, for which dozens of men were flown to Marrakesh. The BBC understands Mr Jeffries and Mr Smith had also invited friends. Alex - who asked for his name to be changed to protect his identity - said he was a struggling model supporting his family back home when he was recruited as a dancer for the event, where he expected he would have to strip.</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2023-10-03 09:56:14</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>approximated</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>https://www.bbc.com/news/world-66990622</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>https://news.google.com/rss/articles/CBMiJ2h0dHBzOi8vd3d3LmJiYy5jb20vbmV3cy93b3JsZC02Njk5MDYyMtIBK2h0dHBzOi8vd3d3LmJiYy5jb20vbmV3cy93b3JsZC02Njk5MDYyMi5hbXA?oc=5</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>https://www.bbc.com</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>BBC</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Are you a robot?</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Why did this happen?
-Please make sure your browser supports JavaScript and cookies and that you are not blocking them from loading. For more information you can review our Terms of Service and Cookie Policy.</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2023-10-03 03:35:41</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>approximated</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>https://news.google.com/rss/articles/CBMicmh0dHBzOi8vd3d3LmJsb29tYmVyZy5jb20vbmV3cy9hcnRpY2xlcy8yMDIzLTEwLTAzL2NoaW5lc2Utc3RvY2tzLWluLWhvbmcta29uZy1zbHVtcC1sZWFkaW5nLWFzaWEtZXF1aXRpZXMtc2VsbG9mZtIBAA?oc=5</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>https://www.bloomberg.com</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Bloomberg</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>First Mover Americas: Bitcoin Hits Highest Price in a Month</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>It is officially trial week for FTX founder Sam Bankman-Fried. It’s been exactly nine months and 20 days since the former crypto CEO got arrested at his then-home in the Bahamas. On Tuesday, he is set to start the trial in which he will win back his freedom, or be locked up for what a federal judge says could be a “very long” time. Thousands of pages of evidence, ranging from internal documents to audio recordings, will be presented and fought over in the next six weeks as U.S. prosecutors try to prove that the former FTX founder knowingly defrauded customers and business partners. Arguably the most damning evidence – or lack thereof – could come from the recollections and personal opinions of Bankman-Fried’s former colleagues, friends and housemates.</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2023-10-02 00:00:00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>parsed</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://www.coindesk.com/markets/2023/10/02/first-mover-americas-bitcoin-hits-highest-price-in-a-month/</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://news.google.com/rss/articles/CBMiZ2h0dHBzOi8vd3d3LmNvaW5kZXNrLmNvbS9tYXJrZXRzLzIwMjMvMTAvMDIvZmlyc3QtbW92ZXItYW1lcmljYXMtYml0Y29pbi1oaXRzLWhpZ2hlc3QtcHJpY2UtaW4tYS1tb250aC_SAXZodHRwczovL3d3dy5jb2luZGVzay5jb20vbWFya2V0cy8yMDIzLzEwLzAyL2ZpcnN0LW1vdmVyLWFtZXJpY2FzLWJpdGNvaW4taGl0cy1oaWdoZXN0LXByaWNlLWluLWEtbW9udGgvP291dHB1dFR5cGU9YW1w?oc=5</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://www.coindesk.com</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>CoinDesk</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Bond investors feel the heat as popular fixed-income ETF suffers lowest close since 2007</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>October is kicking off with a renewed bond-market rout, pushing up yields and sending a popular fixed-income ETF on Monday to its lowest close since the early days of the 2007-2009 financial crisis.
+The iShares 20+ Year Bond ETF TLT, widely known by its “TLT” ticker, dropped 2% to $86.93 a share Monday afternoon, on track for its lowest close since Aug. 20, 2007, according to Dow Jones Market Data. The ETF has dropped 12.7% so far this year.
+Treasurys had rallied to begin 2023, finding support after a brutal 2022 rout that was described as the worst in investors’ lifetimes, with yields surging as the Federal Reserve aggressively hiked interest rates over the course of the year. Bonds rallied earlier this year as the Fed slowed the pace of rate increases, but have seen renewed pressure, driving yields to new highs, as investors pencil in yields remaining elevated.
+Bonds and stocks both stumbled last year, delivering a rare double-whammy to investors who typically look to government debt to cushion the blow in the event of an equity market downturn.
+The S&amp;P 500 SPX remains up 11.7% in the year to date, but suffered consecutive monthly losses in August and September. Gains have been driven largely by an earlier surge for megacap tech stocks. The Dow Jones Industrial Average DJIA is up just 0.9% in the year to date.
+TLT had dropped last week to its lowest since 2008, but then saw a respite as Treasurys bounced ahead of the weekend as worries mounted over the possibility of a U.S. government shutdown.
+But a stopgap funding bill, approved by lawmakers on Saturday, averted a shutdown, leaving investors to return their focus to expectations the Federal Reserve will keep rates elevated for a lengthy period — and may be forced to further tighten policy — in its effort to bring down inflation.
+Bond prices and yields move in opposite directions.
+The yield on the 10-year Treasury note BX:TMUBMUSD10Y jumped more than 10 points to trade above 4.67%, its highest since October 2007.
+See: Stock-market investors focus on rising yields as government shutdown averted
+Bond ETFs matter because they are a popular way for individual investors to gain exposure in the U.S. fixed-income.
+Similarly, the closely followed iShares Core U.S. Aggregate Bond ETF AGG was under further selling pressure on Monday, suffering its lowest close since 2008. It tracks the closely followed U.S. Bloomberg Aggregate Bond Index, the main gauge of performance for investment-grade bonds. It also is the index all fixed-income investors strive to beat each year.
+—Joy Wiltermuth contributed.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2023-10-02 17:50:00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>approximated</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>['William Watts']</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.marketwatch.com/story/renewed-bond-market-selloff-puts-popular-etf-on-track-for-lowest-close-since-2007-6f48db77</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>https://news.google.com/rss/articles/CBMifGh0dHBzOi8vd3d3Lm1hcmtldHdhdGNoLmNvbS9zdG9yeS9yZW5ld2VkLWJvbmQtbWFya2V0LXNlbGxvZmYtcHV0cy1wb3B1bGFyLWV0Zi1vbi10cmFjay1mb3ItbG93ZXN0LWNsb3NlLXNpbmNlLTIwMDctNmY0OGRiNzfSAYABaHR0cHM6Ly93d3cubWFya2V0d2F0Y2guY29tL2FtcC9zdG9yeS9yZW5ld2VkLWJvbmQtbWFya2V0LXNlbGxvZmYtcHV0cy1wb3B1bGFyLWV0Zi1vbi10cmFjay1mb3ItbG93ZXN0LWNsb3NlLXNpbmNlLTIwMDctNmY0OGRiNzc?oc=5</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://www.marketwatch.com</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>MarketWatch</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>China Evergrande’s Founder: From Rags to Riches to Under Investigation</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>Hui Ka Yan founded the real estate behemoth China Evergrande. His promise to transform rural villages to metropolises with middle-class comforts made him one of China’s wealthiest people. He rubbed shoulders with officials in the highest levels of government, celebrating the Communist Party’s 100th anniversary in 2021 at Tiananmen Square.
 Now, he is being investigated by the authorities for suspected criminal behavior.
@@ -1287,92 +1488,49 @@
 Signs of trouble for Mr. Hui’s company surfaced in 2020. China’s red-hot property market started to cool after a campaign by the country’s top leader, Xi Jinping, to slow its growth. And Mr. Xi’s response to the Covid pandemic, ordering lockdowns across the country, reduced spending on properties and started to spook would-be home buyers. In 2021, Evergrande defaulted on payments to some creditors. Its debts piled up.</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>2023-10-02 00:00:00</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>parsed</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>['Tiffany May', 'More About Tiffany May']</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>https://www.nytimes.com/2023/10/02/business/china-evergrande-founder-hui-ka-yan.html</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>https://news.google.com/rss/articles/CBMiVGh0dHBzOi8vd3d3Lm55dGltZXMuY29tLzIwMjMvMTAvMDIvYnVzaW5lc3MvY2hpbmEtZXZlcmdyYW5kZS1mb3VuZGVyLWh1aS1rYS15YW4uaHRtbNIBAA?oc=5</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>https://www.nytimes.com</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>The New York Times</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Apple and Nvidia stock: What the charts show about the tech giants</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>2023-10-03 03:52:15</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>approximated</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=p2kRUPEZlC0</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>https://news.google.com/rss/articles/CCAiC3Aya1JVUEVabEMwmAEB?oc=5</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Yahoo Finance</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Elon Musk’s X Slapped With Trademark Lawsuit From Social Media Ad Agency</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>The Battles of the Xs: Elon Musks’s Twitter Sued Over Name</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>X Corp., the company formerly known as that ditched its bird logo in July, has notched another lawsuit in its growing pile of legal woes.
 That ad agency, X Social Media, sued X. Corp in Florida on Monday, arguing that consumers are likely to to confuse their ad services with the Elon Musk-owned company.
@@ -1385,271 +1543,39 @@
 Despite his lawyers being informed of Brody’s defamation claim in August, Bankston has said that Musk declined to either retract his unfounded accusation or apologize for it.</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>2023-10-03 04:13:45</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>parsed</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>['Charisma Madarang']</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>https://www.rollingstone.com/culture/culture-news/elon-musk-x-trademark-lawsuit-social-media-ad-agency-1234837345/</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>https://news.google.com/rss/articles/CBMicmh0dHBzOi8vd3d3LnJvbGxpbmdzdG9uZS5jb20vY3VsdHVyZS9jdWx0dXJlLW5ld3MvZWxvbi1tdXNrLXgtdHJhZGVtYXJrLWxhd3N1aXQtc29jaWFsLW1lZGlhLWFkLWFnZW5jeS0xMjM0ODM3MzQ1L9IBdmh0dHBzOi8vd3d3LnJvbGxpbmdzdG9uZS5jb20vY3VsdHVyZS9jdWx0dXJlLW5ld3MvZWxvbi1tdXNrLXgtdHJhZGVtYXJrLWxhd3N1aXQtc29jaWFsLW1lZGlhLWFkLWFnZW5jeS0xMjM0ODM3MzQ1L2FtcC8?oc=5</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>https://www.rollingstone.com</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>Rolling Stone</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Taiwan Tech Firms Helping Huawei With China Chip Plants</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>2023-10-03 03:12:22</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>approximated</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=loaqfCqhGZY</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>https://news.google.com/rss/articles/CCAiC2xvYXFmQ3FoR1pZmAEB?oc=5</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Bloomberg Television</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Lilly to Acquire POINT Biopharma to Expand Oncology Capabilities into Next-Generation Radioligand Therapies</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>INDIANAPOLIS, Oct. 3, 2023 /PRNewswire/ -- Eli Lilly and Company (NYSE: LLY) and POINT Biopharma Global, Inc. (NASDAQ: PNT) today announced a definitive agreement for Lilly to acquire POINT, a radiopharmaceutical company with a pipeline of clinical and preclinical-stage radioligand therapies in development for the treatment of cancer. Radioligand therapy can enable the precise targeting of cancer by linking a radioisotope to a targeting molecule that delivers radiation directly to cancer cells, enabling significant anti-tumor efficacy while limiting the impact to healthy tissue.
-POINT's lead programs are in late-phase development. PNT20021 is a prostate-specific membrane antigen (PSMA) targeted radioligand therapy in development for patients with metastatic castration-resistant prostate cancer (mCRPC) after progression on hormonal treatment. Topline data from this study are expected in the fourth quarter of 2023. PNT20031 is a somatostatin receptor (SSTR) targeted radioligand therapy in development for the treatment of patients with gastroenteropancreatic neuroendocrine tumors (GEP-NETs). Beyond the late-stage clinical pipeline, POINT has several additional programs in earlier stages of clinical and preclinical development. Additionally, POINT operates a 180,000-square-foot radiopharmaceutical manufacturing campus in Indianapolis, as well as a radiopharmaceutical research and development center in Toronto. These facilities will be utilized alongside POINT's extensive network of supply chain partners for sourcing radioisotopes and their precursors.
-"Over the past few years, we have seen how well-designed radiopharmaceuticals can demonstrate meaningful results for patients with cancer and rapidly integrate into standards of care, yet the field remains in the early days of the impact it may ultimately deliver," said Jacob Van Naarden, President of Loxo@Lilly, the oncology unit of Eli Lilly and Company. "We are excited by the potential of this emerging modality and see the acquisition of POINT as the beginning of our investment in developing multiple meaningful radioligand medicines for hard-to-treat cancers, as we have done in small molecule and biologic oncology drug discovery and development. We look forward to welcoming POINT colleagues to Lilly and working together to build upon their achievements as we develop a pipeline of meaningful new radioligand treatments for patients."
-Joe McCann, Ph.D., CEO of POINT added: "The combination of POINT's team, infrastructure and capabilities with Lilly's global resources and experience could significantly accelerate the discovery, development and global access to radiopharmaceuticals. I look forward to a future where patients all over the world can benefit from the new cancer treatment options made possible by the joining of our two companies today."
-Terms of the Agreement
-Lilly will commence a tender offer to acquire all outstanding shares of POINT for a purchase price of $12.50 per share in cash (an aggregate of approximately $1.4 billion) payable at closing. The transaction has been approved by the boards of directors of both companies.
-The transaction is not subject to any financing condition and is expected to close near the end of 2023, subject to customary closing conditions, including the tender of a majority of the outstanding shares of POINT's common stock, and license transfer approval from the U.S. Nuclear Regulatory Commission. Following the successful closing of the tender offer, Lilly will acquire any shares of POINT that are not tendered in the tender offer through a second-step merger at the same consideration as paid in the tender offer.
-The purchase price payable at closing represents a premium of approximately 87% to POINT's closing stock price on Oct. 2, 2023, the last trading day before the announcement of the transaction, and 68% to the 30-day volume-weighted average price. POINT's board of directors unanimously recommends that POINT's stockholders tender their shares in the tender offer.
-Lilly will determine the accounting treatment of this transaction as a business combination or an asset acquisition, including any related acquired in-process research and development charges, according to Generally Accepted Accounting Principles (GAAP) upon closing. This transaction will thereafter be reflected in Lilly's financial results and financial guidance.
-For Lilly, Goldman Sachs &amp; Co. LLC is acting as exclusive financial advisor and Kirkland &amp; Ellis LLP is acting as legal counsel. For POINT, Centerview Partners LLC is acting as exclusive financial advisor and Skadden, Arps, Slate, Meagher &amp; Flom LLP is acting as legal counsel.
-About POINT Biopharma Global, Inc.
-POINT Biopharma Global, Inc. is a globally focused radiopharmaceutical company building a platform for the clinical development and commercialization of radioligands that fight cancer. POINT aims to transform precision oncology by combining a portfolio of targeted radioligand assets, a seasoned management team, an industry-leading pipeline, in-house manufacturing capabilities, and secured supply for medical isotopes including actinium-225 and lutetium-177. POINT's active clinical trials include FRONTIER, a phase 1 trial for PNT2004, a pan-cancer program targeting fibroblast activation protein-α (FAP-α), and SPLASH, the phase 3 trial for PNT2002 for people with metastatic castration resistant prostate cancer (mCRPC) after second-line hormonal treatment. Learn more about POINT Biopharma Global, Inc. at pointbiopharma.com.
-About Lilly
-Lilly unites caring with discovery to create medicines that make life better for people around the world. We've been pioneering life-changing discoveries for nearly 150 years, and today our medicines help more than 51 million people across the globe. Harnessing the power of biotechnology, chemistry and genetic medicine, our scientists are urgently advancing new discoveries to solve some of the world's most significant health challenges, redefining diabetes care, treating obesity and curtailing its most devastating long-term effects, advancing the fight against Alzheimer's disease, providing solutions to some of the most debilitating immune system disorders, and transforming the most difficult-to-treat cancers into manageable diseases. With each step toward a healthier world, we're motivated by one thing: making life better for millions more people. That includes delivering innovative clinical trials that reflect the diversity of our world and working to ensure our medicines are accessible and affordable. To learn more, visit Lilly.com and Lilly.com/news or follow us on Facebook, Instagram, Twitter and LinkedIn. C-LLY
-Cautionary Statement Regarding Forward-Looking Statements
-This press release contains forward-looking statements regarding Lilly's proposed acquisition of POINT, including regarding prospective benefits of the proposed acquisition and radioligand therapies, regarding the anticipated occurrence, manner and timing of the proposed tender offer and the closing of the proposed acquisition, regarding the company's product candidates and ongoing clinical and preclinical development, and regarding the accounting treatment of the potential acquisition under GAAP and its potential impact on Lilly's financial results and financial guidance. All statements other than statements of historical fact are statements that could be deemed forward-looking statements. Forward-looking statements reflect current beliefs and expectations; however, these statements involve inherent risks and uncertainties, including with respect to consummating the proposed acquisition and any competing offers or acquisition proposals for POINT, drug research, development and commercialization, Lilly's evaluation of the accounting treatment of the potential acquisition and its potential impact on its financial results and financial guidance, uncertainties as to how many of POINT's stockholders will tender their stock in the tender offer, the effects of the proposed acquisition (or the announcement thereof) on POINT's stock price, relationships with key third parties or governmental entities, transaction costs, risks that the proposed acquisition disrupts current plans and operations or adversely affects employee retention, potentially diverting management's attention from POINT's ongoing business operations, changes in POINT's business during the period between announcement and closing of the proposed acquisition, and any legal proceedings that may be instituted related to the proposed acquisition. Actual results could differ materially due to various factors, risks and uncertainties. Among other things, there can be no guarantee that the proposed acquisition will be completed in the anticipated timeframe or at all, that the conditions required to complete the proposed acquisition will be met, that any event, change or other circumstance that could give rise to the termination of the definitive agreement for the proposed acquisition will not occur, that Lilly will realize the expected benefits of the proposed acquisition, that product candidates will be approved on anticipated timelines or at all, that any products, if approved, will be commercially successful, that Lilly's financial results will be consistent with its expected 2023 guidance or that Lilly can reliably predict the impact of the proposed acquisition on its financial results or financial guidance. For further discussion of these and other risks and uncertainties, see Lilly's and POINT's most recent Form 10-K and Form 10-Q filings with the United States Securities and Exchange Commission (the "SEC"). Except as required by law, neither Lilly nor POINT undertakes any duty to update forward-looking statements to reflect events after the date of this press release.
-Additional Information about the Acquisition and Where to Find It
-The tender offer for the outstanding shares of POINT described in this communication has not yet commenced. This communication is for informational purposes only and is neither an offer to purchase nor a solicitation of an offer to sell any securities, nor is it a substitute for the tender offer materials that Lilly and its acquisition subsidiary will file with the SEC upon commencement of the tender offer. A solicitation and offer to buy outstanding shares of POINT will only be made pursuant to the tender offer materials that Lilly and its acquisition subsidiary intend to file with the SEC. At the time the tender offer is commenced, Lilly and its acquisition subsidiary will file tender offer materials on Schedule TO, and POINT will file a Solicitation/Recommendation Statement on Schedule 14D-9 with the SEC with respect to the tender offer. THE TENDER OFFER MATERIALS (INCLUDING AN OFFER TO PURCHASE, A RELATED LETTER OF TRANSMITTAL AND CERTAIN OTHER TENDER OFFER DOCUMENTS) AND THE SOLICITATION/RECOMMENDATION STATEMENT WILL CONTAIN IMPORTANT INFORMATION ABOUT THE PROPOSED TRANSACTION AND THE PARTIES THERETO. INVESTORS AND STOCKHOLDERS OF POINT ARE URGED TO READ THESE DOCUMENTS CAREFULLY WHEN THEY BECOME AVAILABLE (AND EACH AS IT MAY BE AMENDED OR SUPPLEMENTED FROM TIME TO TIME) BECAUSE THEY WILL CONTAIN IMPORTANT INFORMATION THAT INVESTORS AND STOCKHOLDERS OF POINT SHOULD CONSIDER BEFORE MAKING ANY DECISION REGARDING TENDERING THEIR SHARES OF COMMON STOCK IN THE TENDER OFFER. The tender offer materials (including the Offer to Purchase and the related Letter of Transmittal), as well as the Solicitation/Recommendation Statement, will be made available to all stockholders of POINT at no expense to them at Lilly's website at investor.lilly.com and (once they become available) will be mailed to the stockholders of POINT free of charge. The information contained in, or that can be accessed through, Lilly's website is not a part of, or incorporated by reference herein. The tender offer materials (including the Offer to Purchase and the related Letter of Transmittal), as well as the Solicitation/Recommendation Statement, will also be made available for free on the SEC's website at www.sec.gov. In addition to the Offer to Purchase, the related Letter of Transmittal and certain other tender offer documents, as well as the Solicitation/Recommendation Statement, Lilly and POINT file annual, quarterly, and current reports, proxy statements and other information with the SEC. You may read any reports, statements or other information filed by Lilly and POINT with the SEC for free on the SEC's website at www.sec.gov.
-1 Partnered with Lantheus for exclusive worldwide rights excluding certain territories of: Japan, South Korea, China (including Hong Kong, Macau and Taiwan), Singapore, and Indonesia.
-SOURCE Eli Lilly and Company</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>2023-10-03 10:45:00</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>approximated</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>['Eli Lilly']</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>https://www.prnewswire.com/news-releases/lilly-to-acquire-point-biopharma-to-expand-oncology-capabilities-into-next-generation-radioligand-therapies-301945243.html</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>https://news.google.com/rss/articles/CBMiowFodHRwczovL3d3dy5wcm5ld3N3aXJlLmNvbS9uZXdzLXJlbGVhc2VzL2xpbGx5LXRvLWFjcXVpcmUtcG9pbnQtYmlvcGhhcm1hLXRvLWV4cGFuZC1vbmNvbG9neS1jYXBhYmlsaXRpZXMtaW50by1uZXh0LWdlbmVyYXRpb24tcmFkaW9saWdhbmQtdGhlcmFwaWVzLTMwMTk0NTI0My5odG1s0gEA?oc=5</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>https://www.prnewswire.com</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>PR Newswire</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Self-driving vehicle runs over, pins woman in San Francisco; operator claims human hit her first</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>A woman in San Francisco was found with life-threatening injuries late Monday after being run over and trapped under a self-driving car, authorities said.
-First responders arrived at 5th and Market Streets just after 9:30 p.m. and found the woman underneath the left rear axle of a stopped Cruise autonomous vehicle, San Francisco Fire Capt. Justin Shore told FOX KTVU at the scene.
-"Rescuers did not have any drivers or any passengers to ask about the nature of the injuries or how the victim came to be beneath the vehicle," Shore said.
-Officers rendered aid to the woman and medics rushed to her a hospital for life-threatening injuries, said Officer Robert Rueca, a San Francisco Police Department spokesman.
-CRUISE ROBOTAXI CRASHES INTO FIRETRUCK IN SAN FRANCISCO
-Authorities said that the autonomous vehicle remained on scene and no driver was inside the vehicle at the time of the collision. It was unclear for how long the woman was trapped under the self-driving vehicle.
-"Again, in this unique situation, we had no driver, passengers, nor any witnesses on the sidewalk to tell us how long she had been beneath the vehicle," Shore said.
-Cruise, the company behind the autonomous car, gave an account of what happened in a statement issued on social media early Tuesday. The company that operates the self-driving vehicle said the incident began with a hit-and-run committed by a human driver.
-"At approximately 9:30 pm on October 2, a human-driven vehicle struck a pedestrian while traveling in the lane immediately to the left of a Cruise AV," the statement said. "The initial impact was severe and launched the pedestrian directly in front of the AV."
-CALIFORNIA DMV REQUESTS CRUISE TO HALVE DRIVERLESS CAR FLEET AFTER COLLISION WITH FIRETRUCK IN SAN FRANCISCO
-The driverless Cruise vehicle then "aggressively" hit the brakes "to minimize the impact," the company claimed. Cruise said the driver of the other vehicle fled the scene, while the driverless car remained on site at the request of authorities.
-"Our heartfelt concern and focus is the wellbeing of the person who was injured and we are actively working with police to help identify the responsible driver," the company said.
-The San Francisco Police Department’s Traffic Division is leading the investigation.
-CLICK TO GET THE FOX NEWS APP
-Authorities asked anyone with information about the collision to SFPD at 415-575-4444 or text a tip to TIP411 and begin the message with SFPD.</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>2023-10-03 11:02:00</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>approximated</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>['Stephen Sorace']</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>https://www.foxnews.com/us/self-driving-car-runs-over-pins-woman-san-francisco-operator-claims-human-hit-her-first</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>https://news.google.com/rss/articles/CBMicmh0dHBzOi8vd3d3LmZveG5ld3MuY29tL3VzL3NlbGYtZHJpdmluZy1jYXItcnVucy1vdmVyLXBpbnMtd29tYW4tc2FuLWZyYW5jaXNjby1vcGVyYXRvci1jbGFpbXMtaHVtYW4taGl0LWhlci1maXJzdNIBdmh0dHBzOi8vd3d3LmZveG5ld3MuY29tL3VzL3NlbGYtZHJpdmluZy1jYXItcnVucy1vdmVyLXBpbnMtd29tYW4tc2FuLWZyYW5jaXNjby1vcGVyYXRvci1jbGFpbXMtaHVtYW4taGl0LWhlci1maXJzdC5hbXA?oc=5</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>https://www.foxnews.com</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Fox News</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>10-year Treasury yield reaches highest level in 16 years</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>That was the highest level since Aug. 15, 2007, when it reached 4.745%. The 2-year Treasury yield, which is sensitive to expectations around where the Federal Reserve will set its own key borrowing rate, edged higher to 5.115%.
-As of 8 a.m., the note rose more than 64 basis points to hit 4.727% as investors considered the state of the economy and awaited key data from the labor market that could inform Federal Reserve monetary policy.
-The 10-year Treasury yield, which serves as a benchmark for mortgage rates and as an investor confidence barometer, on Tuesday surged to its highest level since 2007.
-Investors also weighed the Fed's next interest rates moves. Central bank officials have hinted at another rate increase and rates staying elevated for longer since their September meeting.
-Rising yields come even though U.S. lawmakers were able to avoid a government shutdown as they passed a last-minute spending bill on Saturday night. That has bought them time to finish the necessary government funding legislation. A shutdown could have negatively affected the U.S.' credit rating as well as the country's economy.
-In recent public remarks, Fed policymakers have indicated disagreement about whether another rate hike is needed before the end of the year, but concur that rates will have to stay elevated for what could be a prolonged period of time.
-The central bank's Federal Open Market Committee has been using rate increases to bring down inflation that officials consider to be too high even though the rate has come down considerably from its peak in mid-2022.
-"Inflation continues to be too high, and I expect it will likely be appropriate for the Committee to raise rates further and hold them at a restrictive level for some time to return inflation to our 2% goal in a timely way," Fed Governor Michelle Bowman said in prepared remarks Monday.
-Also speaking Monday, Fed Vice Chair for Supervision Michael Barr said it's less important to focus on another hike and more critical to understand that rates likely will remain elevated "for some time." And Cleveland Fed President Loretta Mester, a nonvoter this year on the FOMC, said "we may well need to raise the fed funds rate once more this year and then hold it there for some time."
-Market uncertainty remains about when and whether a rate increase may be implemented. Two central bank policy meetings remain this year, Oct. 31-Nov. 1 and Dec. 12-13. Market pricing Tuesday morning was pointing to just a 25.7% chance of a hike on Nov. 1, but a nearly 45% probability in December, according to futures pricing measured in the CME Group's FedWatch Tool.
-Investors are therefore closely watching both comments from Fed speakers and economic data expected this week.
-The jump in rates has rekindled talk about market "bond vigilantes," a term coined by economist Ed Yardeni to describe the impact when fixed income investors leave the market because of worries over U.S. debt.
-Persistently high fiscal deficits are one factor in the rising costs of borrowing. Public debt has risen past $32.3 trillion this year. Debt has risen to nearly 120% of total gross domestic product.
-"The worry is that the escalating federal budget deficit will create more supply of bonds than demand can meet, requiring higher yields to clear the market; that worry has been the Bond Vigilantes' entrance cue," Yardeni wrote Tuesdaymornning in a note titled "The Bond Vigilante Are On The March."
-"Now the Wild Bunch seems to have taken full control of the Treasury market; we're watching to see if the high-yield market is next," he added. "We are still counting on moderating inflation to stop the beatings in the bond market."
-August's Job Openings and Labor Turnover Survey is due Tuesday and economists surveyed by Dow Jones are expecting it to reflect 8.8 million job openings. Other key data releases this week include September's jobs report on Friday.</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>2023-10-03 00:00:00</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>parsed</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>['Jeff Cox Hakyung Kim Sophie Kiderlin', 'Jeff Cox', 'Hakyung Kim', 'Sophie Kiderlin', 'In']</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>https://www.cnbc.com/2023/10/03/us-treasury-yields-investors-weigh-economic-outlook.html</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>https://news.google.com/rss/articles/CBMiWGh0dHBzOi8vd3d3LmNuYmMuY29tLzIwMjMvMTAvMDMvdXMtdHJlYXN1cnkteWllbGRzLWludmVzdG9ycy13ZWlnaC1lY29ub21pYy1vdXRsb29rLmh0bWzSAVxodHRwczovL3d3dy5jbmJjLmNvbS9hbXAvMjAyMy8xMC8wMy91cy10cmVhc3VyeS15aWVsZHMtaW52ZXN0b3JzLXdlaWdoLWVjb25vbWljLW91dGxvb2suaHRtbA?oc=5</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>https://www.cnbc.com</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>CNBC</t>
         </is>
       </c>
     </row>

</xml_diff>